<commit_message>
APP : Change recurrent value in database and personal data APP : Don't update if same value for recurrent withdraw BUG : Snackbar is not shown when the popup is displayed BUG : Numbers & Durations not translated anymore BUG : Amount in deposit/withdraw not translated in confirmation texts BUG : convertNumberToColumn return A for 1 (should be B), etc
</commit_message>
<xml_diff>
--- a/Data/FiMs Associate.xlsx
+++ b/Data/FiMs Associate.xlsx
@@ -32,7 +32,7 @@
   <commentList>
     <comment authorId="0" ref="A1">
       <text>
-        <t xml:space="preserve">WARNING : Mandatory to know which row to Update when modifying user data</t>
+        <t xml:space="preserve">WARNING : Mandatory to know which row to Update when modifying user data =&gt; SHOULD BE EQUAL TO ROW NUMBER</t>
       </text>
     </comment>
     <comment authorId="0" ref="B1">
@@ -780,7 +780,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="401">
   <si>
     <t>DateTime</t>
   </si>
@@ -1427,10 +1427,10 @@
     <t>Coût si un retrait est effectué avant la fin du mois</t>
   </si>
   <si>
-    <t>Current reccurent amount</t>
+    <t>Current recurrent amount</t>
   </si>
   <si>
-    <t>Current reccurent withdraw amount (will be replaced by the new value)</t>
+    <t>Current recurrent withdraw amount (will be replaced by the new value)</t>
   </si>
   <si>
     <t>Retrait récurrent actuel</t>
@@ -1793,16 +1793,22 @@
     <t>La valeur a été mise à jour !</t>
   </si>
   <si>
-    <t>Value should be at least *</t>
+    <t>Value should be at least * !</t>
   </si>
   <si>
-    <t>La valeur doit être au moins *</t>
+    <t>La valeur doit être au moins * !</t>
   </si>
   <si>
     <t>Value should have at least * character(s) !</t>
   </si>
   <si>
     <t>La valeur doit comporter au moins * caractères</t>
+  </si>
+  <si>
+    <t>The asked recurrent withdraw amount is the same as the current one !</t>
+  </si>
+  <si>
+    <t>Le montant du retrait récurrent demandé est identique à celui en cours</t>
   </si>
   <si>
     <t>Enter your user id</t>
@@ -2611,7 +2617,7 @@
       </c>
       <c r="B1" s="2">
         <f>NOW()</f>
-        <v>44174.94513</v>
+        <v>44175.05717</v>
       </c>
     </row>
     <row r="2">
@@ -2620,7 +2626,7 @@
       </c>
       <c r="B2" s="3">
         <f>DATEVALUE($B$1)</f>
-        <v>44174</v>
+        <v>44175</v>
       </c>
     </row>
     <row r="3">
@@ -2629,7 +2635,7 @@
       </c>
       <c r="B3" s="4">
         <f>TIMEVALUE($B$1)</f>
-        <v>0.9451273148</v>
+        <v>0.05716435185</v>
       </c>
     </row>
     <row r="4">
@@ -2656,7 +2662,7 @@
       </c>
       <c r="B6" s="5">
         <f>DAY($B$1)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
@@ -2665,7 +2671,7 @@
       </c>
       <c r="B7" s="5">
         <f>WEEKDAY($B$1,2)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8">
@@ -2786,7 +2792,7 @@
         <v>26</v>
       </c>
       <c r="O1" s="67" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
     </row>
     <row r="2">
@@ -3910,7 +3916,7 @@
         <v>26</v>
       </c>
       <c r="O1" s="67" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
     </row>
     <row r="2">
@@ -4166,7 +4172,7 @@
         <v>26</v>
       </c>
       <c r="O1" s="67" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
     </row>
     <row r="2">
@@ -4298,7 +4304,7 @@
         <v>26</v>
       </c>
       <c r="O1" s="67" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
     </row>
     <row r="2">
@@ -4430,7 +4436,7 @@
         <v>26</v>
       </c>
       <c r="O1" s="67" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
     </row>
     <row r="2">
@@ -4559,7 +4565,7 @@
         <v>26</v>
       </c>
       <c r="O1" s="67" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
     </row>
     <row r="2">
@@ -4680,8 +4686,8 @@
         <v>Cumulated profit rate</v>
       </c>
       <c r="B4" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.10534831443011654)</f>
-        <v>0.1053483144</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.10531852135476864)</f>
+        <v>0.1053185214</v>
       </c>
     </row>
     <row r="5">
@@ -4700,8 +4706,8 @@
         <v>Cumulated dividend rate</v>
       </c>
       <c r="B6" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.02327811811279844)</f>
-        <v>0.02327811811</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.02327153493459912)</f>
+        <v>0.02327153493</v>
       </c>
     </row>
     <row r="7">
@@ -4720,8 +4726,8 @@
         <v>Saving duration</v>
       </c>
       <c r="B8" s="12">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),9.678302532511978)</f>
-        <v>9.678302533</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),9.681040383299111)</f>
+        <v>9.681040383</v>
       </c>
     </row>
     <row r="9">
@@ -4750,8 +4756,8 @@
         <v>Since Independance duration</v>
       </c>
       <c r="B11" s="13" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"1621 months (135.1 years)")</f>
-        <v>1621 months (135.1 years)</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"1619 months (134.9 years)")</f>
+        <v>1619 months (134.9 years)</v>
       </c>
     </row>
     <row r="12">
@@ -4760,8 +4766,8 @@
         <v>Since Independance gap</v>
       </c>
       <c r="B12" s="10">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),-331998.8550947573)</f>
-        <v>-331998.8551</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),-332177.9915764191)</f>
+        <v>-332177.9916</v>
       </c>
     </row>
     <row r="13">
@@ -4770,8 +4776,8 @@
         <v>Monthly income</v>
       </c>
       <c r="B13" s="10">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1023.4688812125707)</f>
-        <v>1023.468881</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1023.1794386556667)</f>
+        <v>1023.179439</v>
       </c>
     </row>
     <row r="14">
@@ -4790,8 +4796,8 @@
         <v>Income use</v>
       </c>
       <c r="B15" s="14">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.2002326517005606)</f>
-        <v>1.200232652</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.2005721800320177)</f>
+        <v>1.20057218</v>
       </c>
     </row>
     <row r="16">
@@ -4980,8 +4986,8 @@
         <v>Current portfolio duration</v>
       </c>
       <c r="B34" s="12">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),5.122518822724161)</f>
-        <v>5.122518823</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),5.125256673511293)</f>
+        <v>5.125256674</v>
       </c>
     </row>
     <row r="35">
@@ -5040,8 +5046,8 @@
         <v>Current portfolio total profit rate</v>
       </c>
       <c r="B40" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.211620486229803)</f>
-        <v>0.2116204862</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.21150744109827)</f>
+        <v>0.2115074411</v>
       </c>
     </row>
     <row r="41">
@@ -5060,8 +5066,8 @@
         <v>Current portfolio profit rate</v>
       </c>
       <c r="B42" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.19184032104989987)</f>
-        <v>0.191840321</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.19173784224592022)</f>
+        <v>0.1917378422</v>
       </c>
     </row>
     <row r="43">
@@ -5080,8 +5086,8 @@
         <v>Current portfolio dividend rate</v>
       </c>
       <c r="B44" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.040268017527322)</f>
-        <v>0.04026801753</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.040246506834198434)</f>
+        <v>0.04024650683</v>
       </c>
     </row>
     <row r="45">
@@ -5100,8 +5106,8 @@
         <v>Current portfolio cost rate</v>
       </c>
       <c r="B46" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),-0.020487852347418904)</f>
-        <v>-0.02048785235</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),-0.020476907981848702)</f>
+        <v>-0.02047690798</v>
       </c>
     </row>
     <row r="47">
@@ -5227,8 +5233,8 @@
         <v>Investment provision</v>
       </c>
       <c r="B59" s="15">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),-2160.1694938912988)</f>
-        <v>-2160.169494</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),-1964.0223599879537)</f>
+        <v>-1964.02236</v>
       </c>
     </row>
     <row r="60">
@@ -5237,8 +5243,8 @@
         <v>Today's result</v>
       </c>
       <c r="B60" s="15">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),-286.41639999995266)</f>
-        <v>-286.4164</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),-321.2499999999517)</f>
+        <v>-321.25</v>
       </c>
     </row>
     <row r="61">
@@ -5247,8 +5253,8 @@
         <v>Last year daily average progress</v>
       </c>
       <c r="B61" s="15">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),574.4176617875029)</f>
-        <v>574.4176618</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),575.8965525593978)</f>
+        <v>575.8965526</v>
       </c>
     </row>
     <row r="62">
@@ -5257,8 +5263,8 @@
         <v>Transaction per month</v>
       </c>
       <c r="B62" s="20">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),13.89696215139442)</f>
-        <v>13.89696215</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),13.885897691082802)</f>
+        <v>13.88589769</v>
       </c>
     </row>
     <row r="63">
@@ -5267,8 +5273,8 @@
         <v>Average profit per transaction</v>
       </c>
       <c r="B63" s="10">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),363.83804097113097)</f>
-        <v>363.838041</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),364.2301530937424)</f>
+        <v>364.2301531</v>
       </c>
     </row>
     <row r="64">
@@ -5277,8 +5283,8 @@
         <v>Average profit per month</v>
       </c>
       <c r="B64" s="10">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),5056.243484613299)</f>
-        <v>5056.243485</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),5057.662641867133)</f>
+        <v>5057.662642</v>
       </c>
     </row>
     <row r="65">
@@ -5287,8 +5293,8 @@
         <v>Total profit per month</v>
       </c>
       <c r="B65" s="10">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),5458.936680333081)</f>
-        <v>5458.93668</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),5460.355837586915)</f>
+        <v>5460.355838</v>
       </c>
     </row>
     <row r="66">
@@ -5317,8 +5323,8 @@
         <v>Instant profit per month</v>
       </c>
       <c r="B68" s="10">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3997.4954789668045)</f>
-        <v>3997.495479</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3994.312759636417)</f>
+        <v>3994.31276</v>
       </c>
     </row>
     <row r="69">
@@ -5327,8 +5333,8 @@
         <v>Last month stock average progress</v>
       </c>
       <c r="B69" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0016280316010208714)</f>
-        <v>0.001628031601</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0019004604927007913)</f>
+        <v>0.001900460493</v>
       </c>
     </row>
     <row r="70">
@@ -5337,8 +5343,8 @@
         <v>Last negative average profit in days</v>
       </c>
       <c r="B70" s="21" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"7d (0.2m)")</f>
-        <v>7d (0.2m)</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"8d (0.3m)")</f>
+        <v>8d (0.3m)</v>
       </c>
     </row>
     <row r="71">
@@ -5347,8 +5353,8 @@
         <v>Last updated</v>
       </c>
       <c r="B71" s="22">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.19490995370870223)</f>
-        <v>0.1949099537</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.3073569444459281)</f>
+        <v>0.3073569444</v>
       </c>
     </row>
     <row r="72">
@@ -36592,8 +36598,8 @@
     </row>
     <row r="2">
       <c r="A2" s="32">
-        <f t="shared" ref="A2:A7" si="1">ROW()-2</f>
-        <v>0</v>
+        <f t="shared" ref="A2:A7" si="1">ROW()</f>
+        <v>2</v>
       </c>
       <c r="B2" s="32" t="s">
         <v>40</v>
@@ -36682,7 +36688,7 @@
     <row r="3">
       <c r="A3" s="32">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B3" s="32" t="s">
         <v>50</v>
@@ -36777,7 +36783,7 @@
     <row r="4">
       <c r="A4" s="32">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B4" s="32" t="s">
         <v>58</v>
@@ -36860,7 +36866,7 @@
     <row r="5">
       <c r="A5" s="32">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B5" s="32" t="s">
         <v>65</v>
@@ -36951,7 +36957,7 @@
     <row r="6">
       <c r="A6" s="32">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B6" s="32" t="s">
         <v>76</v>
@@ -37042,7 +37048,7 @@
     <row r="7">
       <c r="A7" s="32">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B7" s="32" t="s">
         <v>87</v>
@@ -37942,8 +37948,8 @@
         <v>148</v>
       </c>
       <c r="B26" s="44" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""En date du "" &amp; TO_TEXT(DateTime!$B$6)&amp;""/""&amp;TO_TEXT(DateTime!$B$5)&amp;""/""&amp;TO_TEXT(DateTime!$B$4) &amp; "", "" &amp; COUNT(Associate!$A:$A)-1 &amp; "" personnes. Plus moi, "" &amp; COUNT(Associate!$A:$A) &amp; "" :-)"""),"En date du 9/12/2020, 5 personnes. Plus moi, 6 :-)")</f>
-        <v>En date du 9/12/2020, 5 personnes. Plus moi, 6 :-)</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""En date du "" &amp; TO_TEXT(DateTime!$B$6)&amp;""/""&amp;TO_TEXT(DateTime!$B$5)&amp;""/""&amp;TO_TEXT(DateTime!$B$4) &amp; "", "" &amp; COUNT(Associate!$A:$A)-1 &amp; "" personnes. Plus moi, "" &amp; COUNT(Associate!$A:$A) &amp; "" :-)"""),"En date du 10/12/2020, 5 personnes. Plus moi, 6 :-)")</f>
+        <v>En date du 10/12/2020, 5 personnes. Plus moi, 6 :-)</v>
       </c>
     </row>
     <row r="27">
@@ -38799,11 +38805,11 @@
       <c r="D51" s="50"/>
     </row>
     <row r="52">
-      <c r="A52" s="51" t="s">
+      <c r="A52" s="53" t="s">
         <v>326</v>
       </c>
       <c r="B52" s="50"/>
-      <c r="C52" s="50" t="s">
+      <c r="C52" s="55" t="s">
         <v>327</v>
       </c>
       <c r="D52" s="50"/>
@@ -38819,31 +38825,27 @@
       <c r="D53" s="50"/>
     </row>
     <row r="54">
-      <c r="A54" s="50" t="s">
+      <c r="A54" s="55" t="s">
         <v>330</v>
       </c>
-      <c r="B54" s="51" t="s">
+      <c r="B54" s="51"/>
+      <c r="C54" s="53" t="s">
         <v>331</v>
       </c>
-      <c r="C54" s="51" t="s">
+      <c r="D54" s="50"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="50" t="s">
         <v>332</v>
       </c>
-      <c r="D54" s="50" t="s">
+      <c r="B55" s="51" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="51" t="s">
+      <c r="C55" s="51" t="s">
         <v>334</v>
       </c>
-      <c r="B55" s="51" t="s">
-        <v>331</v>
-      </c>
-      <c r="C55" s="50" t="s">
+      <c r="D55" s="50" t="s">
         <v>335</v>
-      </c>
-      <c r="D55" s="50" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="56">
@@ -38851,24 +38853,28 @@
         <v>336</v>
       </c>
       <c r="B56" s="51" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="C56" s="50" t="s">
         <v>337</v>
       </c>
       <c r="D56" s="50" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="51" t="s">
         <v>338</v>
       </c>
-      <c r="B57" s="50"/>
+      <c r="B57" s="51" t="s">
+        <v>333</v>
+      </c>
       <c r="C57" s="50" t="s">
         <v>339</v>
       </c>
-      <c r="D57" s="50"/>
+      <c r="D57" s="50" t="s">
+        <v>335</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="51" t="s">
@@ -38884,39 +38890,39 @@
       <c r="A59" s="51" t="s">
         <v>342</v>
       </c>
-      <c r="B59" s="50" t="s">
+      <c r="B59" s="50"/>
+      <c r="C59" s="50" t="s">
         <v>343</v>
       </c>
-      <c r="C59" s="50" t="s">
-        <v>344</v>
-      </c>
-      <c r="D59" s="50" t="s">
-        <v>345</v>
-      </c>
+      <c r="D59" s="50"/>
     </row>
     <row r="60">
       <c r="A60" s="51" t="s">
+        <v>344</v>
+      </c>
+      <c r="B60" s="50" t="s">
+        <v>345</v>
+      </c>
+      <c r="C60" s="50" t="s">
         <v>346</v>
       </c>
-      <c r="B60" s="50" t="s">
+      <c r="D60" s="50" t="s">
         <v>347</v>
-      </c>
-      <c r="C60" s="50" t="s">
-        <v>348</v>
-      </c>
-      <c r="D60" s="50" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="51" t="s">
+        <v>348</v>
+      </c>
+      <c r="B61" s="50" t="s">
+        <v>349</v>
+      </c>
+      <c r="C61" s="50" t="s">
         <v>350</v>
       </c>
-      <c r="B61" s="50"/>
-      <c r="C61" s="50" t="s">
+      <c r="D61" s="50" t="s">
         <v>351</v>
       </c>
-      <c r="D61" s="50"/>
     </row>
     <row r="62">
       <c r="A62" s="51" t="s">
@@ -38959,11 +38965,11 @@
       <c r="D65" s="50"/>
     </row>
     <row r="66">
-      <c r="A66" s="50" t="s">
+      <c r="A66" s="51" t="s">
         <v>360</v>
       </c>
-      <c r="B66" s="51"/>
-      <c r="C66" s="51" t="s">
+      <c r="B66" s="50"/>
+      <c r="C66" s="50" t="s">
         <v>361</v>
       </c>
       <c r="D66" s="50"/>
@@ -38984,17 +38990,17 @@
       </c>
       <c r="B68" s="51"/>
       <c r="C68" s="51" t="s">
-        <v>219</v>
+        <v>365</v>
       </c>
       <c r="D68" s="50"/>
     </row>
     <row r="69">
       <c r="A69" s="50" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B69" s="51"/>
       <c r="C69" s="51" t="s">
-        <v>366</v>
+        <v>219</v>
       </c>
       <c r="D69" s="50"/>
     </row>
@@ -39012,39 +39018,39 @@
       <c r="A71" s="50" t="s">
         <v>369</v>
       </c>
-      <c r="B71" s="51" t="s">
+      <c r="B71" s="51"/>
+      <c r="C71" s="51" t="s">
         <v>370</v>
       </c>
-      <c r="C71" s="51" t="s">
-        <v>371</v>
-      </c>
-      <c r="D71" s="50" t="s">
-        <v>372</v>
-      </c>
+      <c r="D71" s="50"/>
     </row>
     <row r="72">
       <c r="A72" s="50" t="s">
+        <v>371</v>
+      </c>
+      <c r="B72" s="51" t="s">
+        <v>372</v>
+      </c>
+      <c r="C72" s="51" t="s">
         <v>373</v>
       </c>
-      <c r="B72" s="51" t="s">
+      <c r="D72" s="50" t="s">
         <v>374</v>
-      </c>
-      <c r="C72" s="51" t="s">
-        <v>369</v>
-      </c>
-      <c r="D72" s="50" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="50" t="s">
+        <v>375</v>
+      </c>
+      <c r="B73" s="51" t="s">
         <v>376</v>
       </c>
-      <c r="B73" s="51"/>
       <c r="C73" s="51" t="s">
+        <v>371</v>
+      </c>
+      <c r="D73" s="50" t="s">
         <v>377</v>
       </c>
-      <c r="D73" s="50"/>
     </row>
     <row r="74">
       <c r="A74" s="50" t="s">
@@ -39057,75 +39063,85 @@
       <c r="D74" s="50"/>
     </row>
     <row r="75">
-      <c r="A75" s="60" t="s">
+      <c r="A75" s="50" t="s">
         <v>380</v>
       </c>
       <c r="B75" s="51"/>
-      <c r="C75" s="50" t="s">
+      <c r="C75" s="51" t="s">
         <v>381</v>
       </c>
-      <c r="D75" s="55" t="s">
+      <c r="D75" s="50"/>
+    </row>
+    <row r="76">
+      <c r="A76" s="60" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="76">
-      <c r="A76" s="50" t="s">
+      <c r="B76" s="51"/>
+      <c r="C76" s="50" t="s">
         <v>383</v>
       </c>
-      <c r="B76" s="51"/>
-      <c r="C76" s="51" t="s">
+      <c r="D76" s="55" t="s">
         <v>384</v>
-      </c>
-      <c r="D76" s="50" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="50" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B77" s="51"/>
       <c r="C77" s="51" t="s">
+        <v>386</v>
+      </c>
+      <c r="D77" s="50" t="s">
         <v>387</v>
       </c>
-      <c r="D77" s="50" t="s">
+    </row>
+    <row r="78">
+      <c r="A78" s="50" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="78">
-      <c r="A78" s="60" t="s">
+      <c r="B78" s="51"/>
+      <c r="C78" s="51" t="s">
         <v>389</v>
       </c>
-      <c r="B78" s="51"/>
-      <c r="C78" s="50" t="s">
+      <c r="D78" s="50" t="s">
         <v>390</v>
-      </c>
-      <c r="D78" s="61" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="60" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B79" s="51"/>
       <c r="C79" s="50" t="s">
+        <v>392</v>
+      </c>
+      <c r="D79" s="61" t="s">
         <v>393</v>
       </c>
-      <c r="D79" s="62" t="s">
+    </row>
+    <row r="80">
+      <c r="A80" s="60" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="80">
-      <c r="A80" s="63" t="s">
+      <c r="B80" s="51"/>
+      <c r="C80" s="50" t="s">
         <v>395</v>
       </c>
-      <c r="B80" s="64"/>
-      <c r="C80" s="65" t="s">
+      <c r="D80" s="62" t="s">
         <v>396</v>
       </c>
-      <c r="D80" s="66" t="s">
+    </row>
+    <row r="81">
+      <c r="A81" s="63" t="s">
         <v>397</v>
+      </c>
+      <c r="B81" s="64"/>
+      <c r="C81" s="65" t="s">
+        <v>398</v>
+      </c>
+      <c r="D81" s="66" t="s">
+        <v>399</v>
       </c>
     </row>
   </sheetData>
@@ -39195,7 +39211,7 @@
         <v>26</v>
       </c>
       <c r="O1" s="67" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
APP : Enlever adresse si vide + Data
</commit_message>
<xml_diff>
--- a/Data/FiMs Associate.xlsx
+++ b/Data/FiMs Associate.xlsx
@@ -690,12 +690,12 @@
         <t xml:space="preserve">Total amount saved</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A68">
+    <comment authorId="0" ref="A69">
       <text>
         <t xml:space="preserve">Sum own by / due to others</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A76">
+    <comment authorId="0" ref="A77">
       <text>
         <t xml:space="preserve">"Variation cumulée" DEGIRO</t>
       </text>
@@ -1105,7 +1105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="981" uniqueCount="510">
   <si>
     <t>DateTime</t>
   </si>
@@ -1844,13 +1844,13 @@
     <t>Date à laquelle a été effectué l'opération</t>
   </si>
   <si>
-    <t>Cost if money is taken before the end of the month</t>
+    <t>Exchange cost for a withdraw (0.5%)</t>
   </si>
   <si>
     <t>Coût de l'opération</t>
   </si>
   <si>
-    <t>Coût si un retrait est effectué avant la fin du mois</t>
+    <t>Coût d'échange pour un retrait (0,5%)</t>
   </si>
   <si>
     <t>Current recurrent amount</t>
@@ -1907,22 +1907,34 @@
     <t>100% backed Security token</t>
   </si>
   <si>
-    <t>Jetons 100% sécurisé, 0% de risque, rendement faible</t>
+    <t>Jetons Sécurité</t>
   </si>
   <si>
-    <t>Jetons 90% sécurisé, 10% de risque, rendement moyen</t>
+    <t>100% sécurisé, 0% de risque, rendement faible</t>
   </si>
   <si>
-    <t>Jetons 10% sécurisé, 90% de risque, rendement important</t>
+    <t>Jetons Sécurité +</t>
   </si>
   <si>
-    <t>Jetons 0% sécurisé, 100% de risque, rendement extrême</t>
+    <t>90% sécurisé, 10% de risque, rendement moyen</t>
+  </si>
+  <si>
+    <t>Jetons Performance</t>
+  </si>
+  <si>
+    <t>10% sécurisé, 90% de risque, rendement important</t>
+  </si>
+  <si>
+    <t>Jetons Performance +</t>
+  </si>
+  <si>
+    <t>0% sécurisé, 100% de risque, rendement extrême</t>
   </si>
   <si>
     <t>Jetons FiMs</t>
   </si>
   <si>
-    <t>Jetons 100% sécurisé permettant la gouvernance de FiMs</t>
+    <t>100% sécurisé, permettant la gouvernance de FiMs</t>
   </si>
   <si>
     <t>Objectif</t>
@@ -2358,6 +2370,12 @@
   </si>
   <si>
     <t>Historique</t>
+  </si>
+  <si>
+    <t>token</t>
+  </si>
+  <si>
+    <t>Jetons</t>
   </si>
   <si>
     <t>personal</t>
@@ -3663,7 +3681,7 @@
       </c>
       <c r="B1" s="2">
         <f>NOW()</f>
-        <v>44869.10664</v>
+        <v>44869.70158</v>
       </c>
     </row>
     <row r="2">
@@ -3681,7 +3699,7 @@
       </c>
       <c r="B3" s="4">
         <f>TIMEVALUE($B$1)</f>
-        <v>0.1066319444</v>
+        <v>0.7015856481</v>
       </c>
     </row>
     <row r="4">
@@ -3760,7 +3778,7 @@
       </c>
       <c r="B12" s="8" t="b">
         <f>AND($B$7&gt;=$B$8,$B$7&lt;=$B$9,$B$3&gt;$B$10,$B$3&lt;$B$11)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3916,10 +3934,10 @@
         <v>183</v>
       </c>
       <c r="C11" s="78" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D11" s="77" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="12">
@@ -3928,10 +3946,10 @@
       </c>
       <c r="B12" s="78"/>
       <c r="C12" s="78" t="s">
-        <v>12</v>
+        <v>186</v>
       </c>
       <c r="D12" s="77" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="13">
@@ -3940,10 +3958,10 @@
       </c>
       <c r="B13" s="78"/>
       <c r="C13" s="78" t="s">
-        <v>13</v>
+        <v>188</v>
       </c>
       <c r="D13" s="77" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
     </row>
     <row r="14">
@@ -3952,10 +3970,10 @@
       </c>
       <c r="B14" s="78"/>
       <c r="C14" s="78" t="s">
-        <v>14</v>
+        <v>190</v>
       </c>
       <c r="D14" s="77" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="15">
@@ -3964,10 +3982,10 @@
       </c>
       <c r="B15" s="78"/>
       <c r="C15" s="78" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="D15" s="77" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
     </row>
     <row r="16">
@@ -3976,10 +3994,10 @@
       </c>
       <c r="B16" s="78"/>
       <c r="C16" s="78" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="D16" s="77" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
     </row>
     <row r="17">
@@ -3991,7 +4009,7 @@
         <v>18</v>
       </c>
       <c r="D17" s="77" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
     <row r="18">
@@ -4000,24 +4018,24 @@
       </c>
       <c r="B18" s="78"/>
       <c r="C18" s="78" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="D18" s="77" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="76" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="B19" s="78" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="C19" s="78" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="D19" s="77" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
     </row>
     <row r="20">
@@ -4025,55 +4043,55 @@
         <v>24</v>
       </c>
       <c r="B20" s="78" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="C20" s="78" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="D20" s="78" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="76" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="B21" s="78" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="C21" s="78" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="D21" s="78" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="76" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="B22" s="77" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="C22" s="77" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="D22" s="77" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="76" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B23" s="77" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="C23" s="77" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="D23" s="77" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
     </row>
     <row r="24">
@@ -4081,27 +4099,27 @@
         <v>26</v>
       </c>
       <c r="B24" s="77" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="C24" s="77" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="D24" s="77" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="76" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="B25" s="77" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="C25" s="77" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="D25" s="77" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
     </row>
     <row r="26">
@@ -4109,13 +4127,13 @@
         <v>30</v>
       </c>
       <c r="B26" s="77" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="C26" s="77" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="D26" s="77" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
     </row>
     <row r="27">
@@ -4123,13 +4141,13 @@
         <v>31</v>
       </c>
       <c r="B27" s="77" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="C27" s="77" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="D27" s="77" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
     </row>
     <row r="28">
@@ -4137,201 +4155,201 @@
         <v>32</v>
       </c>
       <c r="B28" s="77" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="C28" s="77" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="D28" s="79" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="76" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="B29" s="77"/>
       <c r="C29" s="77" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="D29" s="77"/>
     </row>
     <row r="30">
       <c r="A30" s="76" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="B30" s="77"/>
       <c r="C30" s="77" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="D30" s="77"/>
     </row>
     <row r="31">
       <c r="A31" s="76" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="B31" s="77"/>
       <c r="C31" s="77" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="D31" s="77"/>
     </row>
     <row r="32">
       <c r="A32" s="76" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="B32" s="77"/>
       <c r="C32" s="77" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="D32" s="77"/>
     </row>
     <row r="33">
       <c r="A33" s="76" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="B33" s="77"/>
       <c r="C33" s="77" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="D33" s="77"/>
     </row>
     <row r="34">
       <c r="A34" s="76" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="B34" s="77"/>
       <c r="C34" s="77" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="D34" s="80"/>
     </row>
     <row r="35">
       <c r="A35" s="76" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B35" s="77"/>
       <c r="C35" s="77" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="D35" s="80"/>
     </row>
     <row r="36">
       <c r="A36" s="76" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="B36" s="77"/>
       <c r="C36" s="77" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="D36" s="80"/>
     </row>
     <row r="37">
       <c r="A37" s="76" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="B37" s="77"/>
       <c r="C37" s="77" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="D37" s="80"/>
     </row>
     <row r="38">
       <c r="A38" s="76" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="B38" s="77" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="C38" s="77" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="D38" s="77" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="76" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="B39" s="77" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="C39" s="77" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="D39" s="77" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="76" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="B40" s="77" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="C40" s="77" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="D40" s="77" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="76" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="B41" s="77" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="C41" s="76" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="D41" s="77" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="76" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="B42" s="77" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="C42" s="77" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="D42" s="77" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="76" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="B43" s="77" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="C43" s="77" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="D43" s="77" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="76" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="B44" s="77" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="C44" s="77" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="D44" s="77" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
     </row>
     <row r="45">
@@ -4339,13 +4357,13 @@
         <v>1</v>
       </c>
       <c r="B45" s="77" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="C45" s="77" t="s">
         <v>1</v>
       </c>
       <c r="D45" s="77" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
     </row>
     <row r="46">
@@ -4353,153 +4371,153 @@
         <v>37</v>
       </c>
       <c r="B46" s="76" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="C46" s="76" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="D46" s="76" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="76" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="B47" s="77" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="C47" s="77" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="D47" s="77" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="76" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="B48" s="77" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="C48" s="77" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="D48" s="77" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="76" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="B49" s="77" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="C49" s="77" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="D49" s="77" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="76" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="B50" s="77" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="C50" s="77" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="D50" s="77" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="76" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="B51" s="77" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="C51" s="77" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="D51" s="77" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="76" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="B52" s="77" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="C52" s="77" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="D52" s="77" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="76" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="B53" s="77" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="C53" s="77" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="D53" s="77" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="76" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="B54" s="77" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="C54" s="77" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="D54" s="77" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="76" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="B55" s="77" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="C55" s="77" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="D55" s="77" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="76" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="B56" s="77" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="C56" s="77" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="D56" s="77" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
     </row>
     <row r="57">
@@ -4507,41 +4525,41 @@
         <v>25</v>
       </c>
       <c r="B57" s="77" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="C57" s="77" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="D57" s="77" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="76" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="B58" s="77" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="C58" s="77" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="D58" s="77" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="76" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="B59" s="77" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="C59" s="77" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="D59" s="77" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
     </row>
     <row r="60">
@@ -4549,757 +4567,767 @@
         <v>16</v>
       </c>
       <c r="B60" s="77" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="C60" s="77" t="s">
         <v>16</v>
       </c>
       <c r="D60" s="77" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="76" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="B61" s="77"/>
       <c r="C61" s="77" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="D61" s="77"/>
     </row>
     <row r="62">
       <c r="A62" s="76" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="B62" s="79"/>
       <c r="C62" s="79" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="D62" s="77"/>
     </row>
     <row r="63">
       <c r="A63" s="76" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="B63" s="79"/>
       <c r="C63" s="79" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="D63" s="77"/>
     </row>
     <row r="64">
       <c r="A64" s="76" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="B64" s="79"/>
       <c r="C64" s="79" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="D64" s="77"/>
     </row>
     <row r="65">
       <c r="A65" s="76" t="s">
-        <v>337</v>
-      </c>
-      <c r="B65" s="77"/>
-      <c r="C65" s="77" t="s">
-        <v>338</v>
+        <v>341</v>
+      </c>
+      <c r="B65" s="79"/>
+      <c r="C65" s="79" t="s">
+        <v>342</v>
       </c>
       <c r="D65" s="77"/>
     </row>
     <row r="66">
       <c r="A66" s="76" t="s">
-        <v>339</v>
-      </c>
-      <c r="B66" s="77" t="s">
-        <v>340</v>
-      </c>
+        <v>343</v>
+      </c>
+      <c r="B66" s="77"/>
       <c r="C66" s="77" t="s">
-        <v>341</v>
-      </c>
-      <c r="D66" s="77" t="s">
-        <v>342</v>
-      </c>
+        <v>344</v>
+      </c>
+      <c r="D66" s="77"/>
     </row>
     <row r="67">
       <c r="A67" s="76" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="B67" s="77" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="C67" s="77" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="D67" s="77" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="76" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="B68" s="77" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="C68" s="77" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="D68" s="77" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="76" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="B69" s="77" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="C69" s="77" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="D69" s="77" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="76" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B70" s="77" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="C70" s="77" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="D70" s="77" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="76" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="B71" s="77" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="C71" s="77" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="D71" s="77" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="76" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="B72" s="77" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="C72" s="77" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="D72" s="77" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="76" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="B73" s="77" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="C73" s="77" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="D73" s="77" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="76" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="B74" s="77" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="C74" s="77" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="D74" s="77" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="76" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="B75" s="77" t="s">
-        <v>376</v>
-      </c>
-      <c r="C75" s="81" t="s">
-        <v>377</v>
+        <v>378</v>
+      </c>
+      <c r="C75" s="77" t="s">
+        <v>379</v>
       </c>
       <c r="D75" s="77" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="76" t="s">
-        <v>379</v>
-      </c>
-      <c r="B76" s="76" t="s">
-        <v>380</v>
-      </c>
-      <c r="C76" s="76" t="s">
         <v>381</v>
       </c>
-      <c r="D76" s="76" t="s">
+      <c r="B76" s="77" t="s">
         <v>382</v>
+      </c>
+      <c r="C76" s="81" t="s">
+        <v>383</v>
+      </c>
+      <c r="D76" s="77" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="76" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="B77" s="76" t="s">
-        <v>380</v>
-      </c>
-      <c r="C77" s="77" t="s">
-        <v>384</v>
+        <v>386</v>
+      </c>
+      <c r="C77" s="76" t="s">
+        <v>387</v>
       </c>
       <c r="D77" s="76" t="s">
-        <v>382</v>
+        <v>388</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="76" t="s">
-        <v>385</v>
-      </c>
-      <c r="B78" s="77" t="s">
+        <v>389</v>
+      </c>
+      <c r="B78" s="76" t="s">
         <v>386</v>
       </c>
       <c r="C78" s="77" t="s">
-        <v>387</v>
-      </c>
-      <c r="D78" s="77" t="s">
+        <v>390</v>
+      </c>
+      <c r="D78" s="76" t="s">
         <v>388</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="76" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="B79" s="77" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="C79" s="77" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="D79" s="77" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="76" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="B80" s="77" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="C80" s="77" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="D80" s="77" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="76" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="B81" s="77" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="C81" s="77" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="D81" s="77" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="76" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="B82" s="77" t="s">
-        <v>398</v>
+        <v>404</v>
       </c>
       <c r="C82" s="77" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="D82" s="77" t="s">
-        <v>400</v>
+        <v>406</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="76" t="s">
-        <v>403</v>
-      </c>
-      <c r="B83" s="76" t="s">
-        <v>403</v>
+        <v>407</v>
+      </c>
+      <c r="B83" s="77" t="s">
+        <v>404</v>
       </c>
       <c r="C83" s="77" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
       <c r="D83" s="77" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="76" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
       <c r="B84" s="76" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
       <c r="C84" s="77" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="D84" s="77" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="76" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="B85" s="76" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="C85" s="77" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="D85" s="77" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="76" t="s">
-        <v>409</v>
-      </c>
-      <c r="B86" s="77" t="s">
-        <v>410</v>
+        <v>413</v>
+      </c>
+      <c r="B86" s="76" t="s">
+        <v>413</v>
       </c>
       <c r="C86" s="77" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="D86" s="77" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="76" t="s">
-        <v>413</v>
-      </c>
-      <c r="B87" s="77"/>
+        <v>415</v>
+      </c>
+      <c r="B87" s="77" t="s">
+        <v>416</v>
+      </c>
       <c r="C87" s="77" t="s">
-        <v>414</v>
-      </c>
-      <c r="D87" s="77"/>
+        <v>417</v>
+      </c>
+      <c r="D87" s="77" t="s">
+        <v>418</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="76" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="B88" s="77"/>
       <c r="C88" s="77" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="D88" s="77"/>
     </row>
     <row r="89">
       <c r="A89" s="76" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
       <c r="B89" s="77"/>
       <c r="C89" s="77" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="D89" s="77"/>
     </row>
     <row r="90">
       <c r="A90" s="76" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="B90" s="77"/>
       <c r="C90" s="77" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="D90" s="77"/>
     </row>
     <row r="91">
       <c r="A91" s="76" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="B91" s="77"/>
       <c r="C91" s="77" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
       <c r="D91" s="77"/>
     </row>
     <row r="92">
       <c r="A92" s="76" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
       <c r="B92" s="77"/>
       <c r="C92" s="77" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
       <c r="D92" s="77"/>
     </row>
     <row r="93">
       <c r="A93" s="76" t="s">
-        <v>425</v>
-      </c>
-      <c r="B93" s="76"/>
-      <c r="C93" s="76" t="s">
-        <v>426</v>
+        <v>429</v>
+      </c>
+      <c r="B93" s="77"/>
+      <c r="C93" s="77" t="s">
+        <v>430</v>
       </c>
       <c r="D93" s="77"/>
     </row>
     <row r="94">
       <c r="A94" s="76" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="B94" s="76"/>
       <c r="C94" s="76" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="D94" s="77"/>
     </row>
     <row r="95">
       <c r="A95" s="76" t="s">
-        <v>429</v>
-      </c>
-      <c r="B95" s="76" t="s">
-        <v>430</v>
-      </c>
+        <v>433</v>
+      </c>
+      <c r="B95" s="76"/>
       <c r="C95" s="76" t="s">
-        <v>431</v>
-      </c>
-      <c r="D95" s="77" t="s">
-        <v>432</v>
-      </c>
+        <v>434</v>
+      </c>
+      <c r="D95" s="77"/>
     </row>
     <row r="96">
       <c r="A96" s="76" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="B96" s="76" t="s">
-        <v>430</v>
-      </c>
-      <c r="C96" s="77" t="s">
-        <v>434</v>
+        <v>436</v>
+      </c>
+      <c r="C96" s="76" t="s">
+        <v>437</v>
       </c>
       <c r="D96" s="77" t="s">
-        <v>432</v>
+        <v>438</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="76" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
       <c r="B97" s="76" t="s">
-        <v>430</v>
+        <v>436</v>
       </c>
       <c r="C97" s="77" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
       <c r="D97" s="77" t="s">
-        <v>432</v>
+        <v>438</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="76" t="s">
-        <v>437</v>
-      </c>
-      <c r="B98" s="77"/>
+        <v>441</v>
+      </c>
+      <c r="B98" s="76" t="s">
+        <v>436</v>
+      </c>
       <c r="C98" s="77" t="s">
+        <v>442</v>
+      </c>
+      <c r="D98" s="77" t="s">
         <v>438</v>
       </c>
-      <c r="D98" s="77"/>
     </row>
     <row r="99">
       <c r="A99" s="76" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="B99" s="77"/>
       <c r="C99" s="77" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
       <c r="D99" s="77"/>
     </row>
     <row r="100">
       <c r="A100" s="76" t="s">
-        <v>441</v>
-      </c>
-      <c r="B100" s="77" t="s">
-        <v>442</v>
-      </c>
+        <v>445</v>
+      </c>
+      <c r="B100" s="77"/>
       <c r="C100" s="77" t="s">
-        <v>443</v>
-      </c>
-      <c r="D100" s="77" t="s">
-        <v>444</v>
-      </c>
+        <v>446</v>
+      </c>
+      <c r="D100" s="77"/>
     </row>
     <row r="101">
       <c r="A101" s="76" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="B101" s="77" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="C101" s="77" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="D101" s="77" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="76" t="s">
-        <v>449</v>
-      </c>
-      <c r="B102" s="77"/>
+        <v>451</v>
+      </c>
+      <c r="B102" s="77" t="s">
+        <v>452</v>
+      </c>
       <c r="C102" s="77" t="s">
-        <v>450</v>
-      </c>
-      <c r="D102" s="77"/>
+        <v>453</v>
+      </c>
+      <c r="D102" s="77" t="s">
+        <v>454</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" s="76" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
       <c r="B103" s="77"/>
       <c r="C103" s="77" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="D103" s="77"/>
     </row>
     <row r="104">
       <c r="A104" s="76" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="B104" s="77"/>
       <c r="C104" s="77" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
       <c r="D104" s="77"/>
     </row>
     <row r="105">
       <c r="A105" s="76" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
       <c r="B105" s="77"/>
       <c r="C105" s="77" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
       <c r="D105" s="77"/>
     </row>
     <row r="106">
       <c r="A106" s="76" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="B106" s="77"/>
       <c r="C106" s="77" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
       <c r="D106" s="77"/>
     </row>
     <row r="107">
       <c r="A107" s="76" t="s">
-        <v>459</v>
-      </c>
-      <c r="B107" s="76"/>
-      <c r="C107" s="76" t="s">
-        <v>460</v>
+        <v>463</v>
+      </c>
+      <c r="B107" s="77"/>
+      <c r="C107" s="77" t="s">
+        <v>464</v>
       </c>
       <c r="D107" s="77"/>
     </row>
     <row r="108">
       <c r="A108" s="76" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="B108" s="76"/>
       <c r="C108" s="76" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
       <c r="D108" s="77"/>
     </row>
     <row r="109">
       <c r="A109" s="76" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
       <c r="B109" s="76"/>
       <c r="C109" s="76" t="s">
-        <v>197</v>
+        <v>468</v>
       </c>
       <c r="D109" s="77"/>
     </row>
     <row r="110">
       <c r="A110" s="76" t="s">
-        <v>464</v>
+        <v>469</v>
       </c>
       <c r="B110" s="76"/>
       <c r="C110" s="76" t="s">
-        <v>465</v>
+        <v>201</v>
       </c>
       <c r="D110" s="77"/>
     </row>
     <row r="111">
       <c r="A111" s="76" t="s">
-        <v>466</v>
+        <v>470</v>
       </c>
       <c r="B111" s="76"/>
       <c r="C111" s="76" t="s">
-        <v>467</v>
+        <v>471</v>
       </c>
       <c r="D111" s="77"/>
     </row>
     <row r="112">
       <c r="A112" s="76" t="s">
-        <v>468</v>
+        <v>472</v>
       </c>
       <c r="B112" s="76"/>
       <c r="C112" s="76" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
       <c r="D112" s="77"/>
     </row>
     <row r="113">
       <c r="A113" s="76" t="s">
-        <v>470</v>
-      </c>
-      <c r="B113" s="76" t="s">
-        <v>471</v>
-      </c>
+        <v>474</v>
+      </c>
+      <c r="B113" s="76"/>
       <c r="C113" s="76" t="s">
-        <v>472</v>
-      </c>
-      <c r="D113" s="77" t="s">
-        <v>473</v>
-      </c>
+        <v>475</v>
+      </c>
+      <c r="D113" s="77"/>
     </row>
     <row r="114">
       <c r="A114" s="76" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="B114" s="76" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="C114" s="76" t="s">
-        <v>470</v>
+        <v>478</v>
       </c>
       <c r="D114" s="77" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="76" t="s">
-        <v>477</v>
-      </c>
-      <c r="B115" s="76"/>
+        <v>480</v>
+      </c>
+      <c r="B115" s="76" t="s">
+        <v>481</v>
+      </c>
       <c r="C115" s="76" t="s">
-        <v>478</v>
-      </c>
-      <c r="D115" s="77"/>
+        <v>476</v>
+      </c>
+      <c r="D115" s="77" t="s">
+        <v>482</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" s="76" t="s">
-        <v>479</v>
+        <v>483</v>
       </c>
       <c r="B116" s="76"/>
       <c r="C116" s="76" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="D116" s="77"/>
     </row>
     <row r="117">
       <c r="A117" s="76" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
       <c r="B117" s="76"/>
-      <c r="C117" s="77" t="s">
-        <v>482</v>
-      </c>
-      <c r="D117" s="77" t="s">
-        <v>483</v>
-      </c>
+      <c r="C117" s="76" t="s">
+        <v>486</v>
+      </c>
+      <c r="D117" s="77"/>
     </row>
     <row r="118">
       <c r="A118" s="76" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
       <c r="B118" s="76"/>
-      <c r="C118" s="76" t="s">
-        <v>485</v>
+      <c r="C118" s="77" t="s">
+        <v>488</v>
       </c>
       <c r="D118" s="77" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="76" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="B119" s="76"/>
       <c r="C119" s="76" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="D119" s="77" t="s">
-        <v>489</v>
+        <v>492</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="76" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
       <c r="B120" s="76"/>
-      <c r="C120" s="77" t="s">
-        <v>491</v>
-      </c>
-      <c r="D120" s="82" t="s">
-        <v>492</v>
+      <c r="C120" s="76" t="s">
+        <v>494</v>
+      </c>
+      <c r="D120" s="77" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="76" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
       <c r="B121" s="76"/>
       <c r="C121" s="77" t="s">
-        <v>494</v>
+        <v>497</v>
       </c>
       <c r="D121" s="82" t="s">
-        <v>495</v>
+        <v>498</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="76" t="s">
-        <v>496</v>
-      </c>
-      <c r="B122" s="83"/>
-      <c r="C122" s="73" t="s">
-        <v>497</v>
-      </c>
-      <c r="D122" s="84" t="s">
-        <v>498</v>
+        <v>499</v>
+      </c>
+      <c r="B122" s="76"/>
+      <c r="C122" s="77" t="s">
+        <v>500</v>
+      </c>
+      <c r="D122" s="82" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="76" t="s">
+        <v>502</v>
+      </c>
+      <c r="B123" s="83"/>
+      <c r="C123" s="73" t="s">
+        <v>503</v>
+      </c>
+      <c r="D123" s="84" t="s">
+        <v>504</v>
       </c>
     </row>
   </sheetData>
@@ -5332,53 +5360,53 @@
         <v>37</v>
       </c>
       <c r="C1" s="85" t="s">
-        <v>499</v>
+        <v>505</v>
       </c>
       <c r="D1" s="85" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="E1" s="85" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="F1" s="85" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="G1" s="85" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="H1" s="85" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="I1" s="85" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="J1" s="85" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="K1" s="85" t="s">
         <v>25</v>
       </c>
       <c r="L1" s="85" t="s">
-        <v>500</v>
+        <v>506</v>
       </c>
       <c r="M1" s="85" t="s">
-        <v>501</v>
+        <v>507</v>
       </c>
       <c r="N1" s="85" t="s">
         <v>16</v>
       </c>
       <c r="O1" s="85" t="s">
-        <v>502</v>
+        <v>508</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="86">
         <f t="array" ref="A2">IF(ROW()=2,DateTime!$B$1,EOMONTH(INDEX($A:$A,ROW()-1)-1,-1)+1)</f>
-        <v>44869.10664</v>
+        <v>44869.70158</v>
       </c>
       <c r="B2" s="87">
         <f t="array" ref="B2">SUMIFS(Transactions!$C:$C,Transactions!$A:$A,"&gt;"&amp;EOMONTH($A2,-2),Transactions!$A:$A,"&lt;"&amp;$A2,Transactions!$B:$B,$O2,Transactions!$C:$C,"&gt;0")+SUMIFS(Transactions!$C:$C,Transactions!$A:$A,"&gt;="&amp;$A2,Transactions!$A:$A,"&lt;="&amp;EOMONTH($A2,0),Transactions!$B:$B,$O2,Transactions!$D:$D,"&lt;=0",Transactions!$C:$C,"&lt;0")+INDEX($C:$C,ROW()+1)</f>
-        <v>-9781.59</v>
+        <v>0</v>
       </c>
       <c r="C2" s="87">
         <f>MAX($B2+IF($B2&gt;0,SUMIFS(Historic!$G:$G,Historic!$D:$D,"BUY",Historic!$A:$A,"&gt;"&amp;MAX(EOMONTH($A2,-2),MAXIFS(Transactions!$A:$A,Transactions!$A:$A,"&gt;"&amp;EOMONTH($A2,-2),Transactions!$A:$A,"&lt;"&amp;$A2,Transactions!$B:$B,$O2,Transactions!$C:$C,"&gt;0")),Historic!$A:$A,"&lt;"&amp;$A2),0),0)</f>
@@ -5386,11 +5414,11 @@
       </c>
       <c r="D2" s="87">
         <f>$B2-$C2</f>
-        <v>-9781.59</v>
+        <v>0</v>
       </c>
       <c r="E2" s="87">
         <f t="array" ref="E2">INDEX($E:$E,ROW()+1)+$D2</f>
-        <v>-9781.59</v>
+        <v>0</v>
       </c>
       <c r="F2" s="88">
         <v>0.0</v>
@@ -5880,49 +5908,49 @@
         <v>37</v>
       </c>
       <c r="C1" s="85" t="s">
-        <v>499</v>
+        <v>505</v>
       </c>
       <c r="D1" s="85" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="E1" s="85" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="F1" s="85" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="G1" s="85" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="H1" s="85" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="I1" s="85" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="J1" s="85" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="K1" s="85" t="s">
         <v>25</v>
       </c>
       <c r="L1" s="85" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="M1" s="85" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="N1" s="85" t="s">
         <v>16</v>
       </c>
       <c r="O1" s="85" t="s">
-        <v>502</v>
+        <v>508</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="86">
         <f t="array" ref="A2">IF(ROW()=2,DateTime!$B$1,EOMONTH(INDEX($A:$A,ROW()-1)-1,-1)+1)</f>
-        <v>44869.10664</v>
+        <v>44869.70158</v>
       </c>
       <c r="B2" s="87">
         <f t="array" ref="B2">SUMIFS(Transactions!$C:$C,Transactions!$A:$A,"&gt;"&amp;EOMONTH($A2,-2),Transactions!$A:$A,"&lt;"&amp;$A2,Transactions!$B:$B,$O2,Transactions!$C:$C,"&gt;0")+SUMIFS(Transactions!$C:$C,Transactions!$A:$A,"&gt;="&amp;$A2,Transactions!$A:$A,"&lt;="&amp;EOMONTH($A2,0),Transactions!$B:$B,$O2,Transactions!$D:$D,"&lt;=0",Transactions!$C:$C,"&lt;0")+INDEX($C:$C,ROW()+1)</f>
@@ -5942,23 +5970,23 @@
       </c>
       <c r="F2" s="89">
         <f t="array" ref="F2">IF(INDEX($A:$A,ROW()+1),$I2/$N2,0)</f>
-        <v>-0.005627953151</v>
+        <v>0.02566513692</v>
       </c>
       <c r="G2" s="89">
         <f>IF($E2&lt;&gt;0,J2/AVERAGEIF(E2:E62,"&lt;&gt;0"),0)</f>
-        <v>0.3257094478</v>
+        <v>0.3840290352</v>
       </c>
       <c r="H2" s="89">
         <f t="array" ref="H2">IF(INDEX($A:$A,ROW()+1),$G2/(ROWS($A2:$A62)-1)*12,0)</f>
-        <v>0.06514188956</v>
+        <v>0.07680580705</v>
       </c>
       <c r="I2" s="87">
         <f t="array" ref="I2">IF(VLOOKUP($O2,DeFi!$B:$C,2,0)&lt;&gt;"",INDEX($M:$M,ROW())-INDEX($M:$M,ROW()+1),INDEX($N:$N,ROW())-INDEX($N:$N,ROW()+1))</f>
-        <v>-151.2213315</v>
+        <v>711.7627637</v>
       </c>
       <c r="J2" s="87">
         <f>N2-E2</f>
-        <v>4819.685554</v>
+        <v>5682.669649</v>
       </c>
       <c r="K2" s="90">
         <v>0.0</v>
@@ -5968,11 +5996,11 @@
       </c>
       <c r="M2" s="90">
         <f>MAXIFS(DeFi!$I:$I,DeFi!$B:$B,$O2)</f>
-        <v>26869.68555</v>
+        <v>27732.66965</v>
       </c>
       <c r="N2" s="91">
         <f>$M2</f>
-        <v>26869.68555</v>
+        <v>27732.66965</v>
       </c>
       <c r="O2" s="100" t="s">
         <v>47</v>
@@ -8828,49 +8856,49 @@
         <v>37</v>
       </c>
       <c r="C1" s="85" t="s">
-        <v>499</v>
+        <v>505</v>
       </c>
       <c r="D1" s="85" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="E1" s="85" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="F1" s="85" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="G1" s="85" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="H1" s="85" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="I1" s="85" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="J1" s="85" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="K1" s="85" t="s">
         <v>25</v>
       </c>
       <c r="L1" s="85" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="M1" s="85" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="N1" s="85" t="s">
         <v>16</v>
       </c>
       <c r="O1" s="85" t="s">
-        <v>502</v>
+        <v>508</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="86">
         <f t="array" ref="A2">IF(ROW()=2,DateTime!$B$1,EOMONTH(INDEX($A:$A,ROW()-1)-1,-1)+1)</f>
-        <v>44869.10664</v>
+        <v>44869.70158</v>
       </c>
       <c r="B2" s="87">
         <f t="array" ref="B2">SUMIFS(Transactions!$C:$C,Transactions!$A:$A,"&gt;"&amp;EOMONTH($A2,-2),Transactions!$A:$A,"&lt;"&amp;$A2,Transactions!$B:$B,$O2,Transactions!$C:$C,"&gt;0")+SUMIFS(Transactions!$C:$C,Transactions!$A:$A,"&gt;="&amp;$A2,Transactions!$A:$A,"&lt;="&amp;EOMONTH($A2,0),Transactions!$B:$B,$O2,Transactions!$D:$D,"&lt;=0",Transactions!$C:$C,"&lt;0")+INDEX($C:$C,ROW()+1)</f>
@@ -10836,49 +10864,49 @@
         <v>37</v>
       </c>
       <c r="C1" s="85" t="s">
-        <v>499</v>
+        <v>505</v>
       </c>
       <c r="D1" s="85" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="E1" s="85" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="F1" s="85" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="G1" s="85" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="H1" s="85" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="I1" s="85" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="J1" s="85" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="K1" s="85" t="s">
         <v>25</v>
       </c>
       <c r="L1" s="85" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="M1" s="85" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="N1" s="85" t="s">
         <v>16</v>
       </c>
       <c r="O1" s="85" t="s">
-        <v>502</v>
+        <v>508</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="86">
         <f t="array" ref="A2">IF(ROW()=2,DateTime!$B$1,EOMONTH(INDEX($A:$A,ROW()-1)-1,-1)+1)</f>
-        <v>44869.10664</v>
+        <v>44869.70158</v>
       </c>
       <c r="B2" s="87">
         <f t="array" ref="B2">SUMIFS(Transactions!$C:$C,Transactions!$A:$A,"&gt;"&amp;EOMONTH($A2,-2),Transactions!$A:$A,"&lt;"&amp;$A2,Transactions!$B:$B,$O2,Transactions!$C:$C,"&gt;0")+SUMIFS(Transactions!$C:$C,Transactions!$A:$A,"&gt;="&amp;$A2,Transactions!$A:$A,"&lt;="&amp;EOMONTH($A2,0),Transactions!$B:$B,$O2,Transactions!$D:$D,"&lt;=0",Transactions!$C:$C,"&lt;0")+INDEX($C:$C,ROW()+1)</f>
@@ -10898,23 +10926,23 @@
       </c>
       <c r="F2" s="89">
         <f t="array" ref="F2">IF(INDEX($A:$A,ROW()+1),$I2/$N2,0)</f>
-        <v>-0.004871458368</v>
+        <v>0.0196588813</v>
       </c>
       <c r="G2" s="89">
         <f>IF($E2&lt;&gt;0,J2/AVERAGEIF(E2:E28,"&lt;&gt;0"),0)</f>
-        <v>-0.2891188052</v>
+        <v>-0.2668699101</v>
       </c>
       <c r="H2" s="89">
         <f t="array" ref="H2">IF(INDEX($A:$A,ROW()+1),$G2/(ROWS($A2:$A28)-1)*12,0)</f>
-        <v>-0.1334394485</v>
+        <v>-0.1231707277</v>
       </c>
       <c r="I2" s="87">
         <f t="array" ref="I2">IF(VLOOKUP($O2,DeFi!$B:$C,2,0)&lt;&gt;"",INDEX($M:$M,ROW())-INDEX($M:$M,ROW()+1),INDEX($N:$N,ROW())-INDEX($N:$N,ROW()+1))</f>
-        <v>-294.0907538</v>
+        <v>1216.506595</v>
       </c>
       <c r="J2" s="87">
         <f>N2-E2</f>
-        <v>-19629.83328</v>
+        <v>-18119.23593</v>
       </c>
       <c r="K2" s="87">
         <v>0.0</v>
@@ -10924,11 +10952,11 @@
       </c>
       <c r="M2" s="87">
         <f>MAXIFS(DeFi!$I:$I,DeFi!$B:$B,$O2)</f>
-        <v>60370.16672</v>
+        <v>61880.76407</v>
       </c>
       <c r="N2" s="91">
         <f>$M2</f>
-        <v>60370.16672</v>
+        <v>61880.76407</v>
       </c>
       <c r="O2" s="102" t="s">
         <v>46</v>
@@ -12186,49 +12214,49 @@
         <v>37</v>
       </c>
       <c r="C1" s="85" t="s">
-        <v>499</v>
+        <v>505</v>
       </c>
       <c r="D1" s="85" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="E1" s="85" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="F1" s="85" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="G1" s="85" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="H1" s="85" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="I1" s="85" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="J1" s="85" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="K1" s="85" t="s">
         <v>25</v>
       </c>
       <c r="L1" s="85" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="M1" s="85" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="N1" s="85" t="s">
         <v>16</v>
       </c>
       <c r="O1" s="85" t="s">
-        <v>502</v>
+        <v>508</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="86">
         <f t="array" ref="A2">IF(ROW()=2,DateTime!$B$1,EOMONTH(INDEX($A:$A,ROW()-1)-1,-1)+1)</f>
-        <v>44869.10664</v>
+        <v>44869.70158</v>
       </c>
       <c r="B2" s="87">
         <f t="array" ref="B2">SUMIFS(Transactions!$C:$C,Transactions!$A:$A,"&gt;"&amp;EOMONTH($A2,-2),Transactions!$A:$A,"&lt;"&amp;$A2,Transactions!$B:$B,$O2,Transactions!$C:$C,"&gt;0")+SUMIFS(Transactions!$C:$C,Transactions!$A:$A,"&gt;="&amp;$A2,Transactions!$A:$A,"&lt;="&amp;EOMONTH($A2,0),Transactions!$B:$B,$O2,Transactions!$D:$D,"&lt;=0",Transactions!$C:$C,"&lt;0")+INDEX($C:$C,ROW()+1)</f>
@@ -12248,23 +12276,23 @@
       </c>
       <c r="F2" s="89">
         <f t="array" ref="F2">IF(INDEX($A:$A,ROW()+1),$I2/$N2,0)</f>
-        <v>-0.001634491999</v>
+        <v>-0.002448619896</v>
       </c>
       <c r="G2" s="89">
         <f>IF($E2&lt;&gt;0,J2/AVERAGEIF(E2:E26,"&lt;&gt;0"),0)</f>
-        <v>-0.2655417304</v>
+        <v>-0.2661382128</v>
       </c>
       <c r="H2" s="89">
         <f t="array" ref="H2">IF(INDEX($A:$A,ROW()+1),$G2/(ROWS($A2:$A26)-1)*12,0)</f>
-        <v>-0.1327708652</v>
+        <v>-0.1330691064</v>
       </c>
       <c r="I2" s="87">
         <f t="array" ref="I2">IF(VLOOKUP($O2,DeFi!$B:$C,2,0)&lt;&gt;"",INDEX($M:$M,ROW())-INDEX($M:$M,ROW()+1),INDEX($N:$N,ROW())-INDEX($N:$N,ROW()+1))</f>
-        <v>-6.001130362</v>
+        <v>-8.982945916</v>
       </c>
       <c r="J2" s="87">
         <f>N2-E2</f>
-        <v>-1327.44311</v>
+        <v>-1330.424926</v>
       </c>
       <c r="K2" s="87">
         <v>0.0</v>
@@ -12274,11 +12302,11 @@
       </c>
       <c r="M2" s="87">
         <f>MAXIFS(DeFi!$I:$I,DeFi!$B:$B,$O2)</f>
-        <v>3671.55689</v>
+        <v>3668.575074</v>
       </c>
       <c r="N2" s="91">
         <f>$M2</f>
-        <v>3671.55689</v>
+        <v>3668.575074</v>
       </c>
       <c r="O2" s="102" t="s">
         <v>45</v>
@@ -13442,49 +13470,49 @@
         <v>37</v>
       </c>
       <c r="C1" s="85" t="s">
-        <v>499</v>
+        <v>505</v>
       </c>
       <c r="D1" s="85" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="E1" s="85" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="F1" s="85" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="G1" s="85" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="H1" s="85" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="I1" s="85" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="J1" s="85" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="K1" s="85" t="s">
         <v>25</v>
       </c>
       <c r="L1" s="85" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="M1" s="85" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="N1" s="85" t="s">
         <v>16</v>
       </c>
       <c r="O1" s="85" t="s">
-        <v>502</v>
+        <v>508</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="86">
         <f t="array" ref="A2">IF(ROW()=2,DateTime!$B$1,EOMONTH(INDEX($A:$A,ROW()-1)-1,-1)+1)</f>
-        <v>44869.10664</v>
+        <v>44869.70158</v>
       </c>
       <c r="B2" s="87">
         <f t="array" ref="B2">SUMIFS(Transactions!$C:$C,Transactions!$A:$A,"&gt;"&amp;EOMONTH($A2,-2),Transactions!$A:$A,"&lt;"&amp;$A2,Transactions!$B:$B,$O2,Transactions!$C:$C,"&gt;0")+SUMIFS(Transactions!$C:$C,Transactions!$A:$A,"&gt;="&amp;$A2,Transactions!$A:$A,"&lt;="&amp;EOMONTH($A2,0),Transactions!$B:$B,$O2,Transactions!$D:$D,"&lt;=0",Transactions!$C:$C,"&lt;0")+INDEX($C:$C,ROW()+1)</f>
@@ -13504,23 +13532,23 @@
       </c>
       <c r="F2" s="89">
         <f t="array" ref="F2">IF(INDEX($A:$A,ROW()+1),$I2/$N2,0)</f>
-        <v>-0.001634491999</v>
+        <v>-0.002448619896</v>
       </c>
       <c r="G2" s="89">
         <f>IF($E2&lt;&gt;0,J2/AVERAGEIF(E2:E26,"&lt;&gt;0"),0)</f>
-        <v>-0.2655417304</v>
+        <v>-0.2661382128</v>
       </c>
       <c r="H2" s="89">
         <f t="array" ref="H2">IF(INDEX($A:$A,ROW()+1),$G2/(ROWS($A2:$A26)-1)*12,0)</f>
-        <v>-0.1327708652</v>
+        <v>-0.1330691064</v>
       </c>
       <c r="I2" s="87">
         <f t="array" ref="I2">IF(VLOOKUP($O2,DeFi!$B:$C,2,0)&lt;&gt;"",INDEX($M:$M,ROW())-INDEX($M:$M,ROW()+1),INDEX($N:$N,ROW())-INDEX($N:$N,ROW()+1))</f>
-        <v>-6.001130362</v>
+        <v>-8.982945916</v>
       </c>
       <c r="J2" s="87">
         <f>N2-E2</f>
-        <v>-1327.44311</v>
+        <v>-1330.424926</v>
       </c>
       <c r="K2" s="87">
         <v>0.0</v>
@@ -13530,11 +13558,11 @@
       </c>
       <c r="M2" s="87">
         <f>MAXIFS(DeFi!$I:$I,DeFi!$B:$B,$O2)</f>
-        <v>3671.55689</v>
+        <v>3668.575074</v>
       </c>
       <c r="N2" s="91">
         <f>$M2</f>
-        <v>3671.55689</v>
+        <v>3668.575074</v>
       </c>
       <c r="O2" s="102" t="s">
         <v>44</v>
@@ -14698,49 +14726,49 @@
         <v>37</v>
       </c>
       <c r="C1" s="85" t="s">
-        <v>499</v>
+        <v>505</v>
       </c>
       <c r="D1" s="85" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="E1" s="85" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="F1" s="85" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="G1" s="85" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="H1" s="85" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="I1" s="85" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="J1" s="85" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="K1" s="85" t="s">
         <v>25</v>
       </c>
       <c r="L1" s="85" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="M1" s="85" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="N1" s="85" t="s">
         <v>16</v>
       </c>
       <c r="O1" s="85" t="s">
-        <v>502</v>
+        <v>508</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="86">
         <f t="array" ref="A2">IF(ROW()=2,DateTime!$B$1,EOMONTH(INDEX($A:$A,ROW()-1)-1,-1)+1)</f>
-        <v>44869.10664</v>
+        <v>44869.70158</v>
       </c>
       <c r="B2" s="87">
         <f t="array" ref="B2">SUMIFS(Transactions!$C:$C,Transactions!$A:$A,"&gt;"&amp;EOMONTH($A2,-2),Transactions!$A:$A,"&lt;"&amp;$A2,Transactions!$B:$B,$O2,Transactions!$C:$C,"&gt;0")+SUMIFS(Transactions!$C:$C,Transactions!$A:$A,"&gt;="&amp;$A2,Transactions!$A:$A,"&lt;="&amp;EOMONTH($A2,0),Transactions!$B:$B,$O2,Transactions!$D:$D,"&lt;=0",Transactions!$C:$C,"&lt;0")+INDEX($C:$C,ROW()+1)</f>
@@ -14760,23 +14788,23 @@
       </c>
       <c r="F2" s="89">
         <f t="array" ref="F2">IF(INDEX($A:$A,ROW()+1),$I2/$N2,0)</f>
-        <v>-0.005830467574</v>
+        <v>0.02191566465</v>
       </c>
       <c r="G2" s="89">
         <f>IF($E2&lt;&gt;0,J2/AVERAGEIF(E2:E22,"&lt;&gt;0"),0)</f>
-        <v>-0.1716451387</v>
+        <v>-0.1481465071</v>
       </c>
       <c r="H2" s="89">
         <f t="array" ref="H2">IF(INDEX($A:$A,ROW()+1),$G2/(ROWS($A2:$A22)-1)*12,0)</f>
-        <v>-0.1029870832</v>
+        <v>-0.08888790427</v>
       </c>
       <c r="I2" s="87">
         <f t="array" ref="I2">IF(VLOOKUP($O2,DeFi!$B:$C,2,0)&lt;&gt;"",INDEX($M:$M,ROW())-INDEX($M:$M,ROW()+1),INDEX($N:$N,ROW())-INDEX($N:$N,ROW()+1))</f>
-        <v>-24.14848079</v>
+        <v>93.34467739</v>
       </c>
       <c r="J2" s="87">
         <f>N2-E2</f>
-        <v>-858.2256937</v>
+        <v>-740.7325356</v>
       </c>
       <c r="K2" s="87">
         <v>0.0</v>
@@ -14786,11 +14814,11 @@
       </c>
       <c r="M2" s="87">
         <f>MAXIFS(DeFi!$I:$I,DeFi!$B:$B,$O2)</f>
-        <v>4141.774306</v>
+        <v>4259.267464</v>
       </c>
       <c r="N2" s="91">
         <f>$M2</f>
-        <v>4141.774306</v>
+        <v>4259.267464</v>
       </c>
       <c r="O2" s="102" t="s">
         <v>43</v>
@@ -15766,49 +15794,49 @@
         <v>37</v>
       </c>
       <c r="C1" s="85" t="s">
-        <v>499</v>
+        <v>505</v>
       </c>
       <c r="D1" s="85" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="E1" s="85" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="F1" s="85" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="G1" s="85" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="H1" s="85" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="I1" s="85" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="J1" s="85" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="K1" s="85" t="s">
         <v>25</v>
       </c>
       <c r="L1" s="85" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="M1" s="85" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="N1" s="85" t="s">
         <v>16</v>
       </c>
       <c r="O1" s="85" t="s">
-        <v>502</v>
+        <v>508</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="86">
         <f t="array" ref="A2">IF(ROW()=2,DateTime!$B$1,EOMONTH(INDEX($A:$A,ROW()-1)-1,-1)+1)</f>
-        <v>44869.10664</v>
+        <v>44869.70158</v>
       </c>
       <c r="B2" s="87">
         <f t="array" ref="B2">SUMIFS(Transactions!$C:$C,Transactions!$A:$A,"&gt;"&amp;EOMONTH($A2,-2),Transactions!$A:$A,"&lt;"&amp;$A2,Transactions!$B:$B,$O2,Transactions!$C:$C,"&gt;0")+SUMIFS(Transactions!$C:$C,Transactions!$A:$A,"&gt;="&amp;$A2,Transactions!$A:$A,"&lt;="&amp;EOMONTH($A2,0),Transactions!$B:$B,$O2,Transactions!$D:$D,"&lt;=0",Transactions!$C:$C,"&lt;0")+INDEX($C:$C,ROW()+1)</f>
@@ -16270,49 +16298,49 @@
         <v>37</v>
       </c>
       <c r="C1" s="85" t="s">
-        <v>499</v>
+        <v>505</v>
       </c>
       <c r="D1" s="85" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="E1" s="85" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="F1" s="85" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="G1" s="85" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="H1" s="85" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="I1" s="85" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="J1" s="85" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="K1" s="85" t="s">
         <v>25</v>
       </c>
       <c r="L1" s="85" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="M1" s="85" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="N1" s="85" t="s">
         <v>16</v>
       </c>
       <c r="O1" s="85" t="s">
-        <v>502</v>
+        <v>508</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="86">
         <f t="array" ref="A2">IF(ROW()=2,DateTime!$B$1,EOMONTH(INDEX($A:$A,ROW()-1)-1,-1)+1)</f>
-        <v>44869.10664</v>
+        <v>44869.70158</v>
       </c>
       <c r="B2" s="87">
         <f t="array" ref="B2">SUMIFS(Transactions!$C:$C,Transactions!$A:$A,"&gt;"&amp;EOMONTH($A2,-2),Transactions!$A:$A,"&lt;"&amp;$A2,Transactions!$B:$B,$O2,Transactions!$C:$C,"&gt;0")+SUMIFS(Transactions!$C:$C,Transactions!$A:$A,"&gt;="&amp;$A2,Transactions!$A:$A,"&lt;="&amp;EOMONTH($A2,0),Transactions!$B:$B,$O2,Transactions!$D:$D,"&lt;=0",Transactions!$C:$C,"&lt;0")+INDEX($C:$C,ROW()+1)</f>
@@ -16331,23 +16359,23 @@
       </c>
       <c r="F2" s="89">
         <f t="array" ref="F2">IF(INDEX($A:$A,ROW()+1),$I2/$N2,0)</f>
-        <v>-0.09304708993</v>
+        <v>-0.02539418892</v>
       </c>
       <c r="G2" s="89">
         <f>IF($E2&lt;&gt;0,J2/AVERAGEIF(E2:E6,"&lt;&gt;0"),0)</f>
-        <v>-0.2588918561</v>
+        <v>-0.2099954254</v>
       </c>
       <c r="H2" s="89">
         <f t="array" ref="H2">IF(INDEX($A:$A,ROW()+1),$G2/(ROWS($A2:$A6)-1)*12,0)</f>
-        <v>-0.7766755683</v>
+        <v>-0.6299862762</v>
       </c>
       <c r="I2" s="87">
         <f t="array" ref="I2">IF(VLOOKUP($O2,DeFi!$B:$C,2,0)&lt;&gt;"",INDEX($M:$M,ROW())-INDEX($M:$M,ROW()+1),INDEX($N:$N,ROW())-INDEX($N:$N,ROW()+1))</f>
-        <v>-13791.59122</v>
+        <v>-4012.305083</v>
       </c>
       <c r="J2" s="87">
         <f>N2-E2</f>
-        <v>-51778.37122</v>
+        <v>-41999.08508</v>
       </c>
       <c r="K2" s="87">
         <v>0.0</v>
@@ -16357,11 +16385,11 @@
       </c>
       <c r="M2" s="87">
         <f>MAXIFS(DeFi!$I:$I,DeFi!$B:$B,$O2)</f>
-        <v>148221.6288</v>
+        <v>158000.9149</v>
       </c>
       <c r="N2" s="91">
         <f>$M2</f>
-        <v>148221.6288</v>
+        <v>158000.9149</v>
       </c>
       <c r="O2" s="101" t="s">
         <v>41</v>
@@ -16581,8 +16609,8 @@
         <v>Cumulated saving</v>
       </c>
       <c r="B1" s="10">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),146265.65877786966)</f>
-        <v>146265.6588</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),156044.9449171155)</f>
+        <v>156044.9449</v>
       </c>
     </row>
     <row r="2">
@@ -16681,8 +16709,8 @@
         <v>Working free duration</v>
       </c>
       <c r="B11" s="13" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"252 months (21 years)")</f>
-        <v>252 months (21 years)</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"269 months (22.4 years)")</f>
+        <v>269 months (22.4 years)</v>
       </c>
     </row>
     <row r="12">
@@ -16691,8 +16719,8 @@
         <v>Since Independance duration</v>
       </c>
       <c r="B12" s="13" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"80 months (6.7 years)")</f>
-        <v>80 months (6.7 years)</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"72 months (6 years)")</f>
+        <v>72 months (6 years)</v>
       </c>
     </row>
     <row r="13">
@@ -16701,8 +16729,8 @@
         <v>Since Independance gap</v>
       </c>
       <c r="B13" s="10">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),-100343.82383643038)</f>
-        <v>-100343.8238</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),-90564.53769718454)</f>
+        <v>-90564.5377</v>
       </c>
     </row>
     <row r="14">
@@ -16911,7 +16939,7 @@
         <v>Associates</v>
       </c>
       <c r="B34" s="10">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2.0)</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.9999999999999998)</f>
         <v>2</v>
       </c>
     </row>
@@ -17128,8 +17156,8 @@
         <v>Associates interest rate</v>
       </c>
       <c r="B56" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2888.776960922256)</f>
-        <v>2888.776961</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),-12021.88886859223)</f>
+        <v>-12021.88887</v>
       </c>
     </row>
     <row r="57">
@@ -17138,8 +17166,8 @@
         <v>Associates interest</v>
       </c>
       <c r="B57" s="17">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),481.462826820376)</f>
-        <v>481.4628268</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),-2003.6481447653714)</f>
+        <v>-2003.648145</v>
       </c>
     </row>
     <row r="58">
@@ -17298,8 +17326,8 @@
         <v>Last updated</v>
       </c>
       <c r="B73" s="22">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),50.35591016203398)</f>
-        <v>50.35591016</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),50.9517201504641)</f>
+        <v>50.95172015</v>
       </c>
     </row>
     <row r="74">
@@ -18839,49 +18867,49 @@
         <v>37</v>
       </c>
       <c r="C1" s="85" t="s">
-        <v>499</v>
+        <v>505</v>
       </c>
       <c r="D1" s="85" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="E1" s="85" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="F1" s="85" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="G1" s="85" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="H1" s="85" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="I1" s="85" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="J1" s="85" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="K1" s="85" t="s">
         <v>25</v>
       </c>
       <c r="L1" s="85" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="M1" s="85" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="N1" s="85" t="s">
         <v>16</v>
       </c>
       <c r="O1" s="85" t="s">
-        <v>502</v>
+        <v>508</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="86">
         <f t="array" ref="A2">IF(ROW()=2,DateTime!$B$1,EOMONTH(INDEX($A:$A,ROW()-1)-1,-1)+1)</f>
-        <v>44869.10664</v>
+        <v>44869.70158</v>
       </c>
       <c r="B2" s="87">
         <f t="array" ref="B2">SUMIFS(Transactions!$C:$C,Transactions!$A:$A,"&gt;"&amp;EOMONTH($A2,-2),Transactions!$A:$A,"&lt;"&amp;$A2,Transactions!$B:$B,$O2,Transactions!$C:$C,"&gt;0")+SUMIFS(Transactions!$C:$C,Transactions!$A:$A,"&gt;="&amp;$A2,Transactions!$A:$A,"&lt;="&amp;EOMONTH($A2,0),Transactions!$B:$B,$O2,Transactions!$D:$D,"&lt;=0",Transactions!$C:$C,"&lt;0")+INDEX($C:$C,ROW()+1)</f>
@@ -18933,7 +18961,7 @@
         <v>0</v>
       </c>
       <c r="O2" s="101" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
     </row>
   </sheetData>
@@ -58287,19 +58315,19 @@
       </c>
       <c r="I2" s="36">
         <f t="array" ref="I2">SUMPRODUCT(OFFSET($A2,0,3,1,5),TRANSPOSE(OFFSET(Token!$C:$C,ROWS(Token!$C:$C)-5,0)))</f>
-        <v>148221.6288</v>
+        <v>158000.9149</v>
       </c>
       <c r="J2" s="36">
         <f>$I$2-SUM(OFFSET($L:$L,2,0))</f>
-        <v>170994.4151</v>
+        <v>180754.4649</v>
       </c>
       <c r="K2" s="36">
         <f>SUM(OFFSET($K:$K,2,0))</f>
-        <v>-1742.626814</v>
+        <v>-977.1598946</v>
       </c>
       <c r="L2" s="36">
         <f t="shared" ref="L2:L10" si="1">$I2-J2</f>
-        <v>-22772.78633</v>
+        <v>-22753.54996</v>
       </c>
       <c r="M2" s="37">
         <f t="shared" ref="M2:M10" si="2">IF(SUMIF(OFFSET($L:$L,2,0),"&lt;0")&lt;0,MAX($L2/SUMIF(OFFSET($L:$L,2,0),"&lt;0"),0),0)</f>
@@ -58348,15 +58376,15 @@
       </c>
       <c r="I3" s="41">
         <f t="array" ref="I3">SUMPRODUCT(OFFSET($A3,0,3,1,5),TRANSPOSE(OFFSET(Token!$C:$C,ROWS(Token!$C:$C)-5,0)))</f>
-        <v>26869.68555</v>
+        <v>27732.66965</v>
       </c>
       <c r="J3" s="41">
         <f>IF($I3=0,0,IF(ISREF(INDIRECT($B3&amp;"!$A$1")),MAXIFS(INDIRECT($B3&amp;"!$N:$N"),INDIRECT($B3&amp;"!$A:$A"),DATE(2022,8,1))+SUMIFS(Transactions!$C:$C,Transactions!$A:$A,"&gt;"&amp;DATE(2022,9,1),Transactions!$B:$B,$B3)+MIN($K3,0),"#ERROR!"))</f>
-        <v>26869.68555</v>
+        <v>27732.66965</v>
       </c>
       <c r="K3" s="41">
-        <f>IF($I3=0,0,IF(ISREF(INDIRECT($B3&amp;"!$A$1")),$I3-MAXIFS(INDIRECT($B3&amp;"!$M:$M"),INDIRECT($B3&amp;"!$A:$A"),DATE(2022,8,1))-SUMIFS(Transactions!$C:$C,Transactions!$A:$A,"&gt;"&amp;DATE(2022,9,1),Transactions!$B:$B,$B3),"#ERROR!"))</f>
-        <v>-1209.31571</v>
+        <f>IF($I3=0,0,IF(ISREF(INDIRECT($B3&amp;"!$A$1")),$I3-MAXIFS(INDIRECT($B3&amp;"!"&amp;IF($C3&lt;&gt;"","$M:$M","$N:$N")),INDIRECT($B3&amp;"!$A:$A"),DATE(2022,8,1))-SUMIFS(Transactions!$C:$C,Transactions!$A:$A,"&gt;"&amp;DATE(2022,9,1),Transactions!$B:$B,$B3),"#ERROR!"))</f>
+        <v>-346.3316149</v>
       </c>
       <c r="L3" s="41">
         <f t="shared" si="1"/>
@@ -58416,7 +58444,7 @@
         <v>684.6</v>
       </c>
       <c r="K4" s="41">
-        <f>IF($I4=0,0,IF(ISREF(INDIRECT($B4&amp;"!$A$1")),$I4-MAXIFS(INDIRECT($B4&amp;"!$M:$M"),INDIRECT($B4&amp;"!$A:$A"),DATE(2022,8,1))-SUMIFS(Transactions!$C:$C,Transactions!$A:$A,"&gt;"&amp;DATE(2022,9,1),Transactions!$B:$B,$B4),"#ERROR!"))</f>
+        <f>IF($I4=0,0,IF(ISREF(INDIRECT($B4&amp;"!$A$1")),$I4-MAXIFS(INDIRECT($B4&amp;"!"&amp;IF($C4&lt;&gt;"","$M:$M","$N:$N")),INDIRECT($B4&amp;"!$A:$A"),DATE(2022,8,1))-SUMIFS(Transactions!$C:$C,Transactions!$A:$A,"&gt;"&amp;DATE(2022,9,1),Transactions!$B:$B,$B4),"#ERROR!"))</f>
         <v>50.6955456</v>
       </c>
       <c r="L4" s="41">
@@ -58425,7 +58453,7 @@
       </c>
       <c r="M4" s="42">
         <f t="shared" si="2"/>
-        <v>0.005691003205</v>
+        <v>0.005695814509</v>
       </c>
       <c r="N4" s="35">
         <f t="shared" si="3"/>
@@ -58470,15 +58498,15 @@
       </c>
       <c r="I5" s="41">
         <f t="array" ref="I5">SUMPRODUCT(OFFSET($A5,0,3,1,5),TRANSPOSE(OFFSET(Token!$C:$C,ROWS(Token!$C:$C)-5,0)))</f>
-        <v>60370.16672</v>
+        <v>61880.76407</v>
       </c>
       <c r="J5" s="41">
         <f>IF($I5=0,0,IF(ISREF(INDIRECT($B5&amp;"!$A$1")),MAXIFS(INDIRECT($B5&amp;"!$N:$N"),INDIRECT($B5&amp;"!$A:$A"),DATE(2022,8,1))+SUMIFS(Transactions!$C:$C,Transactions!$A:$A,"&gt;"&amp;DATE(2022,9,1),Transactions!$B:$B,$B5)+MIN($K5,0),"#ERROR!"))</f>
-        <v>79366.05446</v>
+        <v>80876.65181</v>
       </c>
       <c r="K5" s="41">
-        <f>IF($I5=0,0,IF(ISREF(INDIRECT($B5&amp;"!$A$1")),$I5-MAXIFS(INDIRECT($B5&amp;"!$M:$M"),INDIRECT($B5&amp;"!$A:$A"),DATE(2022,8,1))-SUMIFS(Transactions!$C:$C,Transactions!$A:$A,"&gt;"&amp;DATE(2022,9,1),Transactions!$B:$B,$B5),"#ERROR!"))</f>
-        <v>-2129.945536</v>
+        <f>IF($I5=0,0,IF(ISREF(INDIRECT($B5&amp;"!$A$1")),$I5-MAXIFS(INDIRECT($B5&amp;"!"&amp;IF($C5&lt;&gt;"","$M:$M","$N:$N")),INDIRECT($B5&amp;"!$A:$A"),DATE(2022,8,1))-SUMIFS(Transactions!$C:$C,Transactions!$A:$A,"&gt;"&amp;DATE(2022,9,1),Transactions!$B:$B,$B5),"#ERROR!"))</f>
+        <v>-619.3481863</v>
       </c>
       <c r="L5" s="41">
         <f t="shared" si="1"/>
@@ -58486,7 +58514,7 @@
       </c>
       <c r="M5" s="42">
         <f t="shared" si="2"/>
-        <v>0.8341485961</v>
+        <v>0.8348538043</v>
       </c>
       <c r="N5" s="35">
         <f t="shared" si="3"/>
@@ -58531,23 +58559,23 @@
       </c>
       <c r="I6" s="41">
         <f t="array" ref="I6">SUMPRODUCT(OFFSET($A6,0,3,1,5),TRANSPOSE(OFFSET(Token!$C:$C,ROWS(Token!$C:$C)-5,0)))</f>
-        <v>3671.55689</v>
+        <v>3668.575074</v>
       </c>
       <c r="J6" s="41">
         <f>IF($I6=0,0,IF(ISREF(INDIRECT($B6&amp;"!$A$1")),MAXIFS(INDIRECT($B6&amp;"!$N:$N"),INDIRECT($B6&amp;"!$A:$A"),DATE(2022,8,1))+SUMIFS(Transactions!$C:$C,Transactions!$A:$A,"&gt;"&amp;DATE(2022,9,1),Transactions!$B:$B,$B6)+MIN($K6,0),"#ERROR!"))</f>
         <v>5096.4805</v>
       </c>
       <c r="K6" s="41">
-        <f>IF($I6=0,0,IF(ISREF(INDIRECT($B6&amp;"!$A$1")),$I6-MAXIFS(INDIRECT($B6&amp;"!$M:$M"),INDIRECT($B6&amp;"!$A:$A"),DATE(2022,8,1))-SUMIFS(Transactions!$C:$C,Transactions!$A:$A,"&gt;"&amp;DATE(2022,9,1),Transactions!$B:$B,$B6),"#ERROR!"))</f>
-        <v>8.234581688</v>
+        <f>IF($I6=0,0,IF(ISREF(INDIRECT($B6&amp;"!$A$1")),$I6-MAXIFS(INDIRECT($B6&amp;"!"&amp;IF($C6&lt;&gt;"","$M:$M","$N:$N")),INDIRECT($B6&amp;"!$A:$A"),DATE(2022,8,1))-SUMIFS(Transactions!$C:$C,Transactions!$A:$A,"&gt;"&amp;DATE(2022,9,1),Transactions!$B:$B,$B6),"#ERROR!"))</f>
+        <v>5.252766134</v>
       </c>
       <c r="L6" s="41">
         <f t="shared" si="1"/>
-        <v>-1424.92361</v>
+        <v>-1427.905426</v>
       </c>
       <c r="M6" s="42">
         <f t="shared" si="2"/>
-        <v>0.06257133358</v>
+        <v>0.06275528118</v>
       </c>
       <c r="N6" s="35">
         <f t="shared" si="3"/>
@@ -58592,23 +58620,23 @@
       </c>
       <c r="I7" s="41">
         <f t="array" ref="I7">SUMPRODUCT(OFFSET($A7,0,3,1,5),TRANSPOSE(OFFSET(Token!$C:$C,ROWS(Token!$C:$C)-5,0)))</f>
-        <v>3671.55689</v>
+        <v>3668.575074</v>
       </c>
       <c r="J7" s="41">
         <f>IF($I7=0,0,IF(ISREF(INDIRECT($B7&amp;"!$A$1")),MAXIFS(INDIRECT($B7&amp;"!$N:$N"),INDIRECT($B7&amp;"!$A:$A"),DATE(2022,8,1))+SUMIFS(Transactions!$C:$C,Transactions!$A:$A,"&gt;"&amp;DATE(2022,9,1),Transactions!$B:$B,$B7)+MIN($K7,0),"#ERROR!"))</f>
         <v>5096.4805</v>
       </c>
       <c r="K7" s="41">
-        <f>IF($I7=0,0,IF(ISREF(INDIRECT($B7&amp;"!$A$1")),$I7-MAXIFS(INDIRECT($B7&amp;"!$M:$M"),INDIRECT($B7&amp;"!$A:$A"),DATE(2022,8,1))-SUMIFS(Transactions!$C:$C,Transactions!$A:$A,"&gt;"&amp;DATE(2022,9,1),Transactions!$B:$B,$B7),"#ERROR!"))</f>
-        <v>8.234581688</v>
+        <f>IF($I7=0,0,IF(ISREF(INDIRECT($B7&amp;"!$A$1")),$I7-MAXIFS(INDIRECT($B7&amp;"!"&amp;IF($C7&lt;&gt;"","$M:$M","$N:$N")),INDIRECT($B7&amp;"!$A:$A"),DATE(2022,8,1))-SUMIFS(Transactions!$C:$C,Transactions!$A:$A,"&gt;"&amp;DATE(2022,9,1),Transactions!$B:$B,$B7),"#ERROR!"))</f>
+        <v>5.252766134</v>
       </c>
       <c r="L7" s="41">
         <f t="shared" si="1"/>
-        <v>-1424.92361</v>
+        <v>-1427.905426</v>
       </c>
       <c r="M7" s="42">
         <f t="shared" si="2"/>
-        <v>0.06257133358</v>
+        <v>0.06275528118</v>
       </c>
       <c r="N7" s="35">
         <f t="shared" si="3"/>
@@ -58653,15 +58681,15 @@
       </c>
       <c r="I8" s="41">
         <f t="array" ref="I8">SUMPRODUCT(OFFSET($A8,0,3,1,5),TRANSPOSE(OFFSET(Token!$C:$C,ROWS(Token!$C:$C)-5,0)))</f>
-        <v>4141.774306</v>
+        <v>4259.267464</v>
       </c>
       <c r="J8" s="41">
         <f>IF($I8=0,0,IF(ISREF(INDIRECT($B8&amp;"!$A$1")),MAXIFS(INDIRECT($B8&amp;"!$N:$N"),INDIRECT($B8&amp;"!$A:$A"),DATE(2022,8,1))+SUMIFS(Transactions!$C:$C,Transactions!$A:$A,"&gt;"&amp;DATE(2022,9,1),Transactions!$B:$B,$B8)+MIN($K8,0),"#ERROR!"))</f>
-        <v>4914.025671</v>
+        <v>5031.518829</v>
       </c>
       <c r="K8" s="41">
-        <f>IF($I8=0,0,IF(ISREF(INDIRECT($B8&amp;"!$A$1")),$I8-MAXIFS(INDIRECT($B8&amp;"!$M:$M"),INDIRECT($B8&amp;"!$A:$A"),DATE(2022,8,1))-SUMIFS(Transactions!$C:$C,Transactions!$A:$A,"&gt;"&amp;DATE(2022,9,1),Transactions!$B:$B,$B8),"#ERROR!"))</f>
-        <v>-164.9743295</v>
+        <f>IF($I8=0,0,IF(ISREF(INDIRECT($B8&amp;"!$A$1")),$I8-MAXIFS(INDIRECT($B8&amp;"!"&amp;IF($C8&lt;&gt;"","$M:$M","$N:$N")),INDIRECT($B8&amp;"!$A:$A"),DATE(2022,8,1))-SUMIFS(Transactions!$C:$C,Transactions!$A:$A,"&gt;"&amp;DATE(2022,9,1),Transactions!$B:$B,$B8),"#ERROR!"))</f>
+        <v>-47.48117132</v>
       </c>
       <c r="L8" s="41">
         <f t="shared" si="1"/>
@@ -58669,7 +58697,7 @@
       </c>
       <c r="M8" s="42">
         <f t="shared" si="2"/>
-        <v>0.03391114961</v>
+        <v>0.03393981886</v>
       </c>
       <c r="N8" s="35">
         <f t="shared" si="3"/>
@@ -58718,7 +58746,7 @@
         <v>0</v>
       </c>
       <c r="K9" s="47">
-        <f>IF($I9=0,0,IF(ISREF(INDIRECT($B9&amp;"!$A$1")),$I9-MAXIFS(INDIRECT($B9&amp;"!$M:$M"),INDIRECT($B9&amp;"!$A:$A"),DATE(2022,8,1))-SUMIFS(Transactions!$C:$C,Transactions!$A:$A,"&gt;"&amp;DATE(2022,9,1),Transactions!$B:$B,$B9),"#ERROR!"))</f>
+        <f>IF($I9=0,0,IF(ISREF(INDIRECT($B9&amp;"!$A$1")),$I9-MAXIFS(INDIRECT($B9&amp;"!"&amp;IF($C9&lt;&gt;"","$M:$M","$N:$N")),INDIRECT($B9&amp;"!$A:$A"),DATE(2022,8,1))-SUMIFS(Transactions!$C:$C,Transactions!$A:$A,"&gt;"&amp;DATE(2022,9,1),Transactions!$B:$B,$B9),"#ERROR!"))</f>
         <v>0</v>
       </c>
       <c r="L9" s="47">
@@ -58773,19 +58801,19 @@
       </c>
       <c r="J10" s="47">
         <f>IF($I10=0,0,IF(ISREF(INDIRECT($B10&amp;"!$A$1")),MAXIFS(INDIRECT($B10&amp;"!$N:$N"),INDIRECT($B10&amp;"!$A:$A"),DATE(2022,8,1))+SUMIFS(Transactions!$C:$C,Transactions!$A:$A,"&gt;"&amp;DATE(2022,9,1),Transactions!$B:$B,$B10)+MIN($K10,0),"#ERROR!"))</f>
-        <v>7525.2</v>
+        <v>7500</v>
       </c>
       <c r="K10" s="47">
-        <f>IF($I10=0,0,IF(ISREF(INDIRECT($B10&amp;"!$A$1")),$I10-MAXIFS(INDIRECT($B10&amp;"!$M:$M"),INDIRECT($B10&amp;"!$A:$A"),DATE(2022,8,1))-SUMIFS(Transactions!$C:$C,Transactions!$A:$A,"&gt;"&amp;DATE(2022,9,1),Transactions!$B:$B,$B10),"#ERROR!"))</f>
-        <v>1694.444052</v>
+        <f>IF($I10=0,0,IF(ISREF(INDIRECT($B10&amp;"!$A$1")),$I10-MAXIFS(INDIRECT($B10&amp;"!"&amp;IF($C10&lt;&gt;"","$M:$M","$N:$N")),INDIRECT($B10&amp;"!$A:$A"),DATE(2022,8,1))-SUMIFS(Transactions!$C:$C,Transactions!$A:$A,"&gt;"&amp;DATE(2022,9,1),Transactions!$B:$B,$B10),"#ERROR!"))</f>
+        <v>-25.2</v>
       </c>
       <c r="L10" s="47">
         <f t="shared" si="1"/>
-        <v>-25.2</v>
+        <v>0</v>
       </c>
       <c r="M10" s="48">
         <f t="shared" si="2"/>
-        <v>0.001106583957</v>
+        <v>0</v>
       </c>
       <c r="N10" s="46">
         <f t="shared" si="3"/>
@@ -58895,8 +58923,8 @@
         <v>Dollar (Circle)</v>
       </c>
       <c r="C3" s="52">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.02)</f>
-        <v>1.02</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.01)</f>
+        <v>1.01</v>
       </c>
       <c r="D3" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"EPjFWdd5AufqSSqeM2qN1xzybapC8G4wEGGkZwyTDt1v")</f>
@@ -58905,8 +58933,8 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="51">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0)</f>
-        <v>0</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),169.802356)</f>
+        <v>169.802356</v>
       </c>
     </row>
     <row r="4">
@@ -58919,8 +58947,8 @@
         <v>Dollar (Tether)</v>
       </c>
       <c r="C4" s="52">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.02)</f>
-        <v>1.02</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.01)</f>
+        <v>1.01</v>
       </c>
       <c r="D4" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Es9vMFrzaCERmJfrF4H2FYD4KCoNkY11McCe8BenwNYB")</f>
@@ -58943,8 +58971,8 @@
         <v>Sol</v>
       </c>
       <c r="C5" s="52">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),31.969886561775624)</f>
-        <v>31.96988656</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),33.96482142676525)</f>
+        <v>33.96482143</v>
       </c>
       <c r="D5" s="50" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"So11111111111111111111111111111111111111112")</f>
@@ -58953,8 +58981,8 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="51">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.34895)</f>
-        <v>0.34895</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.9668552)</f>
+        <v>0.9668552</v>
       </c>
     </row>
     <row r="6">
@@ -58967,8 +58995,8 @@
         <v>Sécurité</v>
       </c>
       <c r="C6" s="52">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.0250825478318137)</f>
-        <v>1.025082548</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.0150327189315018)</f>
+        <v>1.015032719</v>
       </c>
       <c r="D6" s="50" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Je6yu7yHQ4YozsrXtQS5vKteX8rV73yPxMU2muLUX1U")</f>
@@ -58997,20 +59025,20 @@
         <v>Sécurité +</v>
       </c>
       <c r="C7" s="52">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.1530814946115753)</f>
-        <v>1.153081495</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.151545114476687)</f>
+        <v>1.151545114</v>
       </c>
       <c r="D7" s="50" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"86nx2WyrdC6VuWyfdG1gMLiiBduktBTJgToKZAYwcbct")</f>
         <v>86nx2WyrdC6VuWyfdG1gMLiiBduktBTJgToKZAYwcbct</v>
       </c>
       <c r="E7" s="28">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.22911018055655089)</f>
-        <v>0.2291101806</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.24609364557601823)</f>
+        <v>0.2460936456</v>
       </c>
       <c r="F7" s="28">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.13047205354075997)</f>
-        <v>0.1304720535</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.14014367769969005)</f>
+        <v>0.1401436777</v>
       </c>
       <c r="G7" s="51">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0)</f>
@@ -59027,20 +59055,20 @@
         <v>Performance</v>
       </c>
       <c r="C8" s="52">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),39.37402579944174)</f>
-        <v>39.3740258</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),41.901346528223996)</f>
+        <v>41.90134653</v>
       </c>
       <c r="D8" s="50" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"4Hnh1UCC6HLzx9NaGKnTVHR2bANcRrhydumdHCnrT3i2")</f>
         <v>4Hnh1UCC6HLzx9NaGKnTVHR2bANcRrhydumdHCnrT3i2</v>
       </c>
       <c r="E8" s="28">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.2685425773567867)</f>
-        <v>0.2685425774</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.2709447432210813)</f>
+        <v>0.2709447432</v>
       </c>
       <c r="F8" s="28">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.23159729464034995)</f>
-        <v>0.2315972946</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.2336689777265999)</f>
+        <v>0.2336689777</v>
       </c>
       <c r="G8" s="51">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0)</f>
@@ -59057,20 +59085,20 @@
         <v>Performance +</v>
       </c>
       <c r="C9" s="52">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),38.265221585603456)</f>
-        <v>38.26522159</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),40.78986359738478)</f>
+        <v>40.7898636</v>
       </c>
       <c r="D9" s="50" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"DNa849drqW19uBV5X9ohpJ5brRGzq856gk3HDRqveFrA")</f>
         <v>DNa849drqW19uBV5X9ohpJ5brRGzq856gk3HDRqveFrA</v>
       </c>
       <c r="E9" s="28">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.2854088500968116)</f>
-        <v>0.2854088501</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.2912498345862459)</f>
+        <v>0.2912498346</v>
       </c>
       <c r="F9" s="28">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.19691452491278993)</f>
-        <v>0.1969145249</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.20094444439626002)</f>
+        <v>0.2009444444</v>
       </c>
       <c r="G9" s="51">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3873.533789587)</f>
@@ -59210,11 +59238,11 @@
       </c>
       <c r="G2" s="57">
         <f t="shared" ref="G2:G10" si="1">INDIRECT($B2&amp;"!$F2")</f>
-        <v>-0.09304708993</v>
+        <v>-0.02539418892</v>
       </c>
       <c r="H2" s="55">
         <f t="shared" ref="H2:H10" si="2">$G2*IF(ISREF(INDIRECT($B2&amp;"!$A$1")),INDIRECT($B2&amp;"!$N$2"),0)</f>
-        <v>-13791.59122</v>
+        <v>-4012.305083</v>
       </c>
       <c r="I2" s="55" t="str">
         <f>IF(ISREF(INDIRECT($B2&amp;"!$A$1")),ROUNDUP((DateTime!$B$2-MIN(INDIRECT($B2&amp;"!$A:$A")))/365.25*12) &amp; " months (" &amp; ROUNDUP((DateTime!$B$2-MIN(INDIRECT($B2&amp;"!$A:$A")))/365.25,1) &amp;  " years)",)</f>
@@ -59230,15 +59258,15 @@
       </c>
       <c r="L2" s="55">
         <f t="shared" ref="L2:L10" si="3">IF(ISREF(INDIRECT($B2&amp;"!$A$1")),INDIRECT($B2&amp;"!J2"),"#ERROR!")</f>
-        <v>-51778.37122</v>
+        <v>-41999.08508</v>
       </c>
       <c r="M2" s="57">
         <f t="shared" ref="M2:M10" si="4">IF(ISREF(INDIRECT($B2&amp;"!$A$1")),INDIRECT($B2&amp;"!H2"),"#ERROR!")</f>
-        <v>-0.7766755683</v>
+        <v>-0.6299862762</v>
       </c>
       <c r="N2" s="58">
         <f t="shared" ref="N2:N10" si="5">SUM($J2:$L2)</f>
-        <v>148221.6288</v>
+        <v>158000.9149</v>
       </c>
       <c r="O2" s="59" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"fdefroco@gmail.com")</f>
@@ -59271,11 +59299,11 @@
       </c>
       <c r="G3" s="57">
         <f t="shared" si="1"/>
-        <v>-0.005627953151</v>
+        <v>0.02566513692</v>
       </c>
       <c r="H3" s="55">
         <f t="shared" si="2"/>
-        <v>-151.2213315</v>
+        <v>711.7627637</v>
       </c>
       <c r="I3" s="55" t="str">
         <f>IF(ISREF(INDIRECT($B3&amp;"!$A$1")),ROUNDUP((DateTime!$B$2-MIN(INDIRECT($B3&amp;"!$A:$A")))/365.25*12) &amp; " months (" &amp; ROUNDUP((DateTime!$B$2-MIN(INDIRECT($B3&amp;"!$A:$A")))/365.25,1) &amp;  " years)",)</f>
@@ -59291,15 +59319,15 @@
       </c>
       <c r="L3" s="55">
         <f t="shared" si="3"/>
-        <v>4819.685554</v>
+        <v>5682.669649</v>
       </c>
       <c r="M3" s="57">
         <f t="shared" si="4"/>
-        <v>0.06514188956</v>
+        <v>0.07680580705</v>
       </c>
       <c r="N3" s="58">
         <f t="shared" si="5"/>
-        <v>26869.68555</v>
+        <v>27732.66965</v>
       </c>
       <c r="O3" s="59" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"isadeloenzien@gmail.com")</f>
@@ -59393,11 +59421,11 @@
       </c>
       <c r="G5" s="57">
         <f t="shared" si="1"/>
-        <v>-0.004871458368</v>
+        <v>0.0196588813</v>
       </c>
       <c r="H5" s="55">
         <f t="shared" si="2"/>
-        <v>-294.0907538</v>
+        <v>1216.506595</v>
       </c>
       <c r="I5" s="55" t="str">
         <f>IF(ISREF(INDIRECT($B5&amp;"!$A$1")),ROUNDUP((DateTime!$B$2-MIN(INDIRECT($B5&amp;"!$A:$A")))/365.25*12) &amp; " months (" &amp; ROUNDUP((DateTime!$B$2-MIN(INDIRECT($B5&amp;"!$A:$A")))/365.25,1) &amp;  " years)",)</f>
@@ -59413,15 +59441,15 @@
       </c>
       <c r="L5" s="55">
         <f t="shared" si="3"/>
-        <v>-19629.83328</v>
+        <v>-18119.23593</v>
       </c>
       <c r="M5" s="57">
         <f t="shared" si="4"/>
-        <v>-0.1334394485</v>
+        <v>-0.1231707277</v>
       </c>
       <c r="N5" s="58">
         <f t="shared" si="5"/>
-        <v>60370.16672</v>
+        <v>61880.76407</v>
       </c>
       <c r="O5" s="59" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"philippe.deregel@live.fr")</f>
@@ -59454,11 +59482,11 @@
       </c>
       <c r="G6" s="57">
         <f t="shared" si="1"/>
-        <v>-0.001634491999</v>
+        <v>-0.002448619896</v>
       </c>
       <c r="H6" s="55">
         <f t="shared" si="2"/>
-        <v>-6.001130362</v>
+        <v>-8.982945916</v>
       </c>
       <c r="I6" s="55" t="str">
         <f>IF(ISREF(INDIRECT($B6&amp;"!$A$1")),ROUNDUP((DateTime!$B$2-MIN(INDIRECT($B6&amp;"!$A:$A")))/365.25*12) &amp; " months (" &amp; ROUNDUP((DateTime!$B$2-MIN(INDIRECT($B6&amp;"!$A:$A")))/365.25,1) &amp;  " years)",)</f>
@@ -59474,15 +59502,15 @@
       </c>
       <c r="L6" s="55">
         <f t="shared" si="3"/>
-        <v>-1327.44311</v>
+        <v>-1330.424926</v>
       </c>
       <c r="M6" s="57">
         <f t="shared" si="4"/>
-        <v>-0.1327708652</v>
+        <v>-0.1330691064</v>
       </c>
       <c r="N6" s="58">
         <f t="shared" si="5"/>
-        <v>3671.55689</v>
+        <v>3668.575074</v>
       </c>
       <c r="O6" s="59" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"futurlizd@yahoo.fr")</f>
@@ -59515,11 +59543,11 @@
       </c>
       <c r="G7" s="57">
         <f t="shared" si="1"/>
-        <v>-0.001634491999</v>
+        <v>-0.002448619896</v>
       </c>
       <c r="H7" s="55">
         <f t="shared" si="2"/>
-        <v>-6.001130362</v>
+        <v>-8.982945916</v>
       </c>
       <c r="I7" s="55" t="str">
         <f>IF(ISREF(INDIRECT($B7&amp;"!$A$1")),ROUNDUP((DateTime!$B$2-MIN(INDIRECT($B7&amp;"!$A:$A")))/365.25*12) &amp; " months (" &amp; ROUNDUP((DateTime!$B$2-MIN(INDIRECT($B7&amp;"!$A:$A")))/365.25,1) &amp;  " years)",)</f>
@@ -59535,15 +59563,15 @@
       </c>
       <c r="L7" s="55">
         <f t="shared" si="3"/>
-        <v>-1327.44311</v>
+        <v>-1330.424926</v>
       </c>
       <c r="M7" s="57">
         <f t="shared" si="4"/>
-        <v>-0.1327708652</v>
+        <v>-0.1330691064</v>
       </c>
       <c r="N7" s="58">
         <f t="shared" si="5"/>
-        <v>3671.55689</v>
+        <v>3668.575074</v>
       </c>
       <c r="O7" s="59" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"mezzo78000@gmail.com")</f>
@@ -59576,11 +59604,11 @@
       </c>
       <c r="G8" s="57">
         <f t="shared" si="1"/>
-        <v>-0.005830467574</v>
+        <v>0.02191566465</v>
       </c>
       <c r="H8" s="55">
         <f t="shared" si="2"/>
-        <v>-24.14848079</v>
+        <v>93.34467739</v>
       </c>
       <c r="I8" s="55" t="str">
         <f>IF(ISREF(INDIRECT($B8&amp;"!$A$1")),ROUNDUP((DateTime!$B$2-MIN(INDIRECT($B8&amp;"!$A:$A")))/365.25*12) &amp; " months (" &amp; ROUNDUP((DateTime!$B$2-MIN(INDIRECT($B8&amp;"!$A:$A")))/365.25,1) &amp;  " years)",)</f>
@@ -59596,15 +59624,15 @@
       </c>
       <c r="L8" s="55">
         <f t="shared" si="3"/>
-        <v>-858.2256937</v>
+        <v>-740.7325356</v>
       </c>
       <c r="M8" s="57">
         <f t="shared" si="4"/>
-        <v>-0.1029870832</v>
+        <v>-0.08888790427</v>
       </c>
       <c r="N8" s="58">
         <f t="shared" si="5"/>
-        <v>4141.774306</v>
+        <v>4259.267464</v>
       </c>
       <c r="O8" s="59" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"didier.villain245@orange.fr")</f>
@@ -59625,7 +59653,7 @@
       </c>
       <c r="D9" s="55">
         <f>IF(ISREF(INDIRECT($B9&amp;"!$A$1")),INDIRECT($B9&amp;"!$K$2")+SUMIFS(Transactions!$D:$D,Transactions!$A:$A,"&gt;"&amp;EOMONTH(DateTime!$B$2,-1),Transactions!$B:$B,$B9),0)</f>
-        <v>-48.90795</v>
+        <v>48.90795</v>
       </c>
       <c r="E9" s="55">
         <f>SUMIFS(Transactions!$C:$C,Transactions!$B:$B,$B9,Transactions!$D:$D,"&gt;0")</f>
@@ -59653,7 +59681,7 @@
       </c>
       <c r="K9" s="55">
         <f>SUMIFS(Transactions!$C:$C,Transactions!$B:$B,$B9,Transactions!$C:$C,"&lt;0",Transactions!$D:$D,"&lt;=0")</f>
-        <v>-33958.6</v>
+        <v>-24177.01</v>
       </c>
       <c r="L9" s="55">
         <f t="shared" si="3"/>
@@ -59665,7 +59693,7 @@
       </c>
       <c r="N9" s="58">
         <f t="shared" si="5"/>
-        <v>1041.4</v>
+        <v>10822.99</v>
       </c>
       <c r="O9" s="59" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"lafalconiere@free.fr")</f>
@@ -59788,8 +59816,8 @@
         <v>-9781.59</v>
       </c>
       <c r="D2" s="55">
-        <f>C2*0.5%</f>
-        <v>-48.90795</v>
+        <f>-C2*0.5%</f>
+        <v>48.90795</v>
       </c>
     </row>
     <row r="3">
@@ -60926,8 +60954,8 @@
       <c r="B22" s="66" t="str">
         <f>"Non, la preuve : en ce moment, le taux d'intérêt moyen des associés est de &lt;b&gt;" &amp; SUBSTITUTE(AVERAGE(Associate!M3:M58),".",",") &amp; "&lt;/b&gt;.&lt;br&gt;
 L'intérêt le plus bas est de &lt;b&gt;" &amp; SUBSTITUTE(MAX(MIN(Associate!M3:M58),1.2%),".",",") &amp; "&lt;/b&gt; et le plus haut de &lt;b&gt;" &amp; SUBSTITUTE(MAX(Associate!M3:M58),".",",") &amp; "&lt;/b&gt;."</f>
-        <v>Non, la preuve : en ce moment, le taux d'intérêt moyen des associés est de &lt;b&gt;-5,84%&lt;/b&gt;.&lt;br&gt;
-L'intérêt le plus bas est de &lt;b&gt;1,20%&lt;/b&gt; et le plus haut de &lt;b&gt;6,51%&lt;/b&gt;.</v>
+        <v>Non, la preuve : en ce moment, le taux d'intérêt moyen des associés est de &lt;b&gt;-5,40%&lt;/b&gt;.&lt;br&gt;
+L'intérêt le plus bas est de &lt;b&gt;1,20%&lt;/b&gt; et le plus haut de &lt;b&gt;7,68%&lt;/b&gt;.</v>
       </c>
     </row>
     <row r="23">
@@ -60952,7 +60980,7 @@
       </c>
       <c r="B25" s="65" t="str">
         <f>"En effet, au pire tu gagnes 1,20% par an, en moyenne "&amp;ROUNDUP(AVERAGE(Associate!M3:M58),2)*100&amp;"% par an, au mieux, "&amp;ROUNDUP(MAX(Associate!M3:M58),2)*100&amp;"% par an."</f>
-        <v>En effet, au pire tu gagnes 1,20% par an, en moyenne -6% par an, au mieux, 7% par an.</v>
+        <v>En effet, au pire tu gagnes 1,20% par an, en moyenne -6% par an, au mieux, 8% par an.</v>
       </c>
     </row>
     <row r="26">
@@ -60990,7 +61018,7 @@
 Et dans les trois cas, 0 € pour moi."</f>
         <v>Au pire des cas, c’est à dire 1,20% de rendement au bout d’un an, cela fait 108 € pour toi et 12 € pour ton association.&lt;br&gt;
 Dans le cas courant, c’est à dire -6% de rendement au bout d’un an, cela fait -540 € pour toi et -60 € pour ton association.&lt;br&gt;
-Au meilleur des cas, c’est à dire 7% de rendement au bout d’un an, cela fait 630. € pour toi et 70 € pour ton association.&lt;br&gt;
+Au meilleur des cas, c’est à dire 8% de rendement au bout d’un an, cela fait 720 € pour toi et 80 € pour ton association.&lt;br&gt;
 Et dans les trois cas, 0 € pour moi.</v>
       </c>
     </row>

</xml_diff>